<commit_message>
Refactoring squib_helpers out, other bonus tweaks
</commit_message>
<xml_diff>
--- a/deck.xlsx
+++ b/deck.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="146">
   <si>
     <t>Type</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>Bonus2Num</t>
+  </si>
+  <si>
+    <t>take wood or metal</t>
   </si>
 </sst>
 </file>
@@ -1117,24 +1120,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1211,6 +1196,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2582,8 +2585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -2591,16 +2594,16 @@
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.3984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="99" customWidth="1"/>
+    <col min="4" max="4" width="4.5" style="93" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="4.59765625" style="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.19921875" style="99" customWidth="1"/>
+    <col min="9" max="9" width="9.19921875" style="93" customWidth="1"/>
     <col min="10" max="10" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="99" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" style="93" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
@@ -2608,17 +2611,17 @@
     <col min="18" max="255" width="6.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="87" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:255" s="81" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="103" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="94" t="s">
+      <c r="C1" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="88" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -2630,305 +2633,305 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="110" t="s">
+      <c r="H1" s="104" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="94" t="s">
+      <c r="I1" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="85" t="s">
+      <c r="K1" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="88" t="s">
+      <c r="L1" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="94" t="s">
+      <c r="M1" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="85" t="s">
+      <c r="N1" s="79" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="85" t="s">
+      <c r="O1" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="85" t="s">
+      <c r="P1" s="79" t="s">
         <v>144</v>
       </c>
-      <c r="Q1" s="85" t="s">
+      <c r="Q1" s="79" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="86"/>
-      <c r="AG1" s="86"/>
-      <c r="AH1" s="86"/>
-      <c r="AI1" s="86"/>
-      <c r="AJ1" s="86"/>
-      <c r="AK1" s="86"/>
-      <c r="AL1" s="86"/>
-      <c r="AM1" s="86"/>
-      <c r="AN1" s="86"/>
-      <c r="AO1" s="86"/>
-      <c r="AP1" s="86"/>
-      <c r="AQ1" s="86"/>
-      <c r="AR1" s="86"/>
-      <c r="AS1" s="86"/>
-      <c r="AT1" s="86"/>
-      <c r="AU1" s="86"/>
-      <c r="AV1" s="86"/>
-      <c r="AW1" s="86"/>
-      <c r="AX1" s="86"/>
-      <c r="AY1" s="86"/>
-      <c r="AZ1" s="86"/>
-      <c r="BA1" s="86"/>
-      <c r="BB1" s="86"/>
-      <c r="BC1" s="86"/>
-      <c r="BD1" s="86"/>
-      <c r="BE1" s="86"/>
-      <c r="BF1" s="86"/>
-      <c r="BG1" s="86"/>
-      <c r="BH1" s="86"/>
-      <c r="BI1" s="86"/>
-      <c r="BJ1" s="86"/>
-      <c r="BK1" s="86"/>
-      <c r="BL1" s="86"/>
-      <c r="BM1" s="86"/>
-      <c r="BN1" s="86"/>
-      <c r="BO1" s="86"/>
-      <c r="BP1" s="86"/>
-      <c r="BQ1" s="86"/>
-      <c r="BR1" s="86"/>
-      <c r="BS1" s="86"/>
-      <c r="BT1" s="86"/>
-      <c r="BU1" s="86"/>
-      <c r="BV1" s="86"/>
-      <c r="BW1" s="86"/>
-      <c r="BX1" s="86"/>
-      <c r="BY1" s="86"/>
-      <c r="BZ1" s="86"/>
-      <c r="CA1" s="86"/>
-      <c r="CB1" s="86"/>
-      <c r="CC1" s="86"/>
-      <c r="CD1" s="86"/>
-      <c r="CE1" s="86"/>
-      <c r="CF1" s="86"/>
-      <c r="CG1" s="86"/>
-      <c r="CH1" s="86"/>
-      <c r="CI1" s="86"/>
-      <c r="CJ1" s="86"/>
-      <c r="CK1" s="86"/>
-      <c r="CL1" s="86"/>
-      <c r="CM1" s="86"/>
-      <c r="CN1" s="86"/>
-      <c r="CO1" s="86"/>
-      <c r="CP1" s="86"/>
-      <c r="CQ1" s="86"/>
-      <c r="CR1" s="86"/>
-      <c r="CS1" s="86"/>
-      <c r="CT1" s="86"/>
-      <c r="CU1" s="86"/>
-      <c r="CV1" s="86"/>
-      <c r="CW1" s="86"/>
-      <c r="CX1" s="86"/>
-      <c r="CY1" s="86"/>
-      <c r="CZ1" s="86"/>
-      <c r="DA1" s="86"/>
-      <c r="DB1" s="86"/>
-      <c r="DC1" s="86"/>
-      <c r="DD1" s="86"/>
-      <c r="DE1" s="86"/>
-      <c r="DF1" s="86"/>
-      <c r="DG1" s="86"/>
-      <c r="DH1" s="86"/>
-      <c r="DI1" s="86"/>
-      <c r="DJ1" s="86"/>
-      <c r="DK1" s="86"/>
-      <c r="DL1" s="86"/>
-      <c r="DM1" s="86"/>
-      <c r="DN1" s="86"/>
-      <c r="DO1" s="86"/>
-      <c r="DP1" s="86"/>
-      <c r="DQ1" s="86"/>
-      <c r="DR1" s="86"/>
-      <c r="DS1" s="86"/>
-      <c r="DT1" s="86"/>
-      <c r="DU1" s="86"/>
-      <c r="DV1" s="86"/>
-      <c r="DW1" s="86"/>
-      <c r="DX1" s="86"/>
-      <c r="DY1" s="86"/>
-      <c r="DZ1" s="86"/>
-      <c r="EA1" s="86"/>
-      <c r="EB1" s="86"/>
-      <c r="EC1" s="86"/>
-      <c r="ED1" s="86"/>
-      <c r="EE1" s="86"/>
-      <c r="EF1" s="86"/>
-      <c r="EG1" s="86"/>
-      <c r="EH1" s="86"/>
-      <c r="EI1" s="86"/>
-      <c r="EJ1" s="86"/>
-      <c r="EK1" s="86"/>
-      <c r="EL1" s="86"/>
-      <c r="EM1" s="86"/>
-      <c r="EN1" s="86"/>
-      <c r="EO1" s="86"/>
-      <c r="EP1" s="86"/>
-      <c r="EQ1" s="86"/>
-      <c r="ER1" s="86"/>
-      <c r="ES1" s="86"/>
-      <c r="ET1" s="86"/>
-      <c r="EU1" s="86"/>
-      <c r="EV1" s="86"/>
-      <c r="EW1" s="86"/>
-      <c r="EX1" s="86"/>
-      <c r="EY1" s="86"/>
-      <c r="EZ1" s="86"/>
-      <c r="FA1" s="86"/>
-      <c r="FB1" s="86"/>
-      <c r="FC1" s="86"/>
-      <c r="FD1" s="86"/>
-      <c r="FE1" s="86"/>
-      <c r="FF1" s="86"/>
-      <c r="FG1" s="86"/>
-      <c r="FH1" s="86"/>
-      <c r="FI1" s="86"/>
-      <c r="FJ1" s="86"/>
-      <c r="FK1" s="86"/>
-      <c r="FL1" s="86"/>
-      <c r="FM1" s="86"/>
-      <c r="FN1" s="86"/>
-      <c r="FO1" s="86"/>
-      <c r="FP1" s="86"/>
-      <c r="FQ1" s="86"/>
-      <c r="FR1" s="86"/>
-      <c r="FS1" s="86"/>
-      <c r="FT1" s="86"/>
-      <c r="FU1" s="86"/>
-      <c r="FV1" s="86"/>
-      <c r="FW1" s="86"/>
-      <c r="FX1" s="86"/>
-      <c r="FY1" s="86"/>
-      <c r="FZ1" s="86"/>
-      <c r="GA1" s="86"/>
-      <c r="GB1" s="86"/>
-      <c r="GC1" s="86"/>
-      <c r="GD1" s="86"/>
-      <c r="GE1" s="86"/>
-      <c r="GF1" s="86"/>
-      <c r="GG1" s="86"/>
-      <c r="GH1" s="86"/>
-      <c r="GI1" s="86"/>
-      <c r="GJ1" s="86"/>
-      <c r="GK1" s="86"/>
-      <c r="GL1" s="86"/>
-      <c r="GM1" s="86"/>
-      <c r="GN1" s="86"/>
-      <c r="GO1" s="86"/>
-      <c r="GP1" s="86"/>
-      <c r="GQ1" s="86"/>
-      <c r="GR1" s="86"/>
-      <c r="GS1" s="86"/>
-      <c r="GT1" s="86"/>
-      <c r="GU1" s="86"/>
-      <c r="GV1" s="86"/>
-      <c r="GW1" s="86"/>
-      <c r="GX1" s="86"/>
-      <c r="GY1" s="86"/>
-      <c r="GZ1" s="86"/>
-      <c r="HA1" s="86"/>
-      <c r="HB1" s="86"/>
-      <c r="HC1" s="86"/>
-      <c r="HD1" s="86"/>
-      <c r="HE1" s="86"/>
-      <c r="HF1" s="86"/>
-      <c r="HG1" s="86"/>
-      <c r="HH1" s="86"/>
-      <c r="HI1" s="86"/>
-      <c r="HJ1" s="86"/>
-      <c r="HK1" s="86"/>
-      <c r="HL1" s="86"/>
-      <c r="HM1" s="86"/>
-      <c r="HN1" s="86"/>
-      <c r="HO1" s="86"/>
-      <c r="HP1" s="86"/>
-      <c r="HQ1" s="86"/>
-      <c r="HR1" s="86"/>
-      <c r="HS1" s="86"/>
-      <c r="HT1" s="86"/>
-      <c r="HU1" s="86"/>
-      <c r="HV1" s="86"/>
-      <c r="HW1" s="86"/>
-      <c r="HX1" s="86"/>
-      <c r="HY1" s="86"/>
-      <c r="HZ1" s="86"/>
-      <c r="IA1" s="86"/>
-      <c r="IB1" s="86"/>
-      <c r="IC1" s="86"/>
-      <c r="ID1" s="86"/>
-      <c r="IE1" s="86"/>
-      <c r="IF1" s="86"/>
-      <c r="IG1" s="86"/>
-      <c r="IH1" s="86"/>
-      <c r="II1" s="86"/>
-      <c r="IJ1" s="86"/>
-      <c r="IK1" s="86"/>
-      <c r="IL1" s="86"/>
-      <c r="IM1" s="86"/>
-      <c r="IN1" s="86"/>
-      <c r="IO1" s="86"/>
-      <c r="IP1" s="86"/>
-      <c r="IQ1" s="86"/>
-      <c r="IR1" s="86"/>
-      <c r="IS1" s="86"/>
-      <c r="IT1" s="86"/>
-      <c r="IU1" s="86"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80"/>
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="80"/>
+      <c r="AI1" s="80"/>
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="80"/>
+      <c r="AM1" s="80"/>
+      <c r="AN1" s="80"/>
+      <c r="AO1" s="80"/>
+      <c r="AP1" s="80"/>
+      <c r="AQ1" s="80"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="80"/>
+      <c r="AT1" s="80"/>
+      <c r="AU1" s="80"/>
+      <c r="AV1" s="80"/>
+      <c r="AW1" s="80"/>
+      <c r="AX1" s="80"/>
+      <c r="AY1" s="80"/>
+      <c r="AZ1" s="80"/>
+      <c r="BA1" s="80"/>
+      <c r="BB1" s="80"/>
+      <c r="BC1" s="80"/>
+      <c r="BD1" s="80"/>
+      <c r="BE1" s="80"/>
+      <c r="BF1" s="80"/>
+      <c r="BG1" s="80"/>
+      <c r="BH1" s="80"/>
+      <c r="BI1" s="80"/>
+      <c r="BJ1" s="80"/>
+      <c r="BK1" s="80"/>
+      <c r="BL1" s="80"/>
+      <c r="BM1" s="80"/>
+      <c r="BN1" s="80"/>
+      <c r="BO1" s="80"/>
+      <c r="BP1" s="80"/>
+      <c r="BQ1" s="80"/>
+      <c r="BR1" s="80"/>
+      <c r="BS1" s="80"/>
+      <c r="BT1" s="80"/>
+      <c r="BU1" s="80"/>
+      <c r="BV1" s="80"/>
+      <c r="BW1" s="80"/>
+      <c r="BX1" s="80"/>
+      <c r="BY1" s="80"/>
+      <c r="BZ1" s="80"/>
+      <c r="CA1" s="80"/>
+      <c r="CB1" s="80"/>
+      <c r="CC1" s="80"/>
+      <c r="CD1" s="80"/>
+      <c r="CE1" s="80"/>
+      <c r="CF1" s="80"/>
+      <c r="CG1" s="80"/>
+      <c r="CH1" s="80"/>
+      <c r="CI1" s="80"/>
+      <c r="CJ1" s="80"/>
+      <c r="CK1" s="80"/>
+      <c r="CL1" s="80"/>
+      <c r="CM1" s="80"/>
+      <c r="CN1" s="80"/>
+      <c r="CO1" s="80"/>
+      <c r="CP1" s="80"/>
+      <c r="CQ1" s="80"/>
+      <c r="CR1" s="80"/>
+      <c r="CS1" s="80"/>
+      <c r="CT1" s="80"/>
+      <c r="CU1" s="80"/>
+      <c r="CV1" s="80"/>
+      <c r="CW1" s="80"/>
+      <c r="CX1" s="80"/>
+      <c r="CY1" s="80"/>
+      <c r="CZ1" s="80"/>
+      <c r="DA1" s="80"/>
+      <c r="DB1" s="80"/>
+      <c r="DC1" s="80"/>
+      <c r="DD1" s="80"/>
+      <c r="DE1" s="80"/>
+      <c r="DF1" s="80"/>
+      <c r="DG1" s="80"/>
+      <c r="DH1" s="80"/>
+      <c r="DI1" s="80"/>
+      <c r="DJ1" s="80"/>
+      <c r="DK1" s="80"/>
+      <c r="DL1" s="80"/>
+      <c r="DM1" s="80"/>
+      <c r="DN1" s="80"/>
+      <c r="DO1" s="80"/>
+      <c r="DP1" s="80"/>
+      <c r="DQ1" s="80"/>
+      <c r="DR1" s="80"/>
+      <c r="DS1" s="80"/>
+      <c r="DT1" s="80"/>
+      <c r="DU1" s="80"/>
+      <c r="DV1" s="80"/>
+      <c r="DW1" s="80"/>
+      <c r="DX1" s="80"/>
+      <c r="DY1" s="80"/>
+      <c r="DZ1" s="80"/>
+      <c r="EA1" s="80"/>
+      <c r="EB1" s="80"/>
+      <c r="EC1" s="80"/>
+      <c r="ED1" s="80"/>
+      <c r="EE1" s="80"/>
+      <c r="EF1" s="80"/>
+      <c r="EG1" s="80"/>
+      <c r="EH1" s="80"/>
+      <c r="EI1" s="80"/>
+      <c r="EJ1" s="80"/>
+      <c r="EK1" s="80"/>
+      <c r="EL1" s="80"/>
+      <c r="EM1" s="80"/>
+      <c r="EN1" s="80"/>
+      <c r="EO1" s="80"/>
+      <c r="EP1" s="80"/>
+      <c r="EQ1" s="80"/>
+      <c r="ER1" s="80"/>
+      <c r="ES1" s="80"/>
+      <c r="ET1" s="80"/>
+      <c r="EU1" s="80"/>
+      <c r="EV1" s="80"/>
+      <c r="EW1" s="80"/>
+      <c r="EX1" s="80"/>
+      <c r="EY1" s="80"/>
+      <c r="EZ1" s="80"/>
+      <c r="FA1" s="80"/>
+      <c r="FB1" s="80"/>
+      <c r="FC1" s="80"/>
+      <c r="FD1" s="80"/>
+      <c r="FE1" s="80"/>
+      <c r="FF1" s="80"/>
+      <c r="FG1" s="80"/>
+      <c r="FH1" s="80"/>
+      <c r="FI1" s="80"/>
+      <c r="FJ1" s="80"/>
+      <c r="FK1" s="80"/>
+      <c r="FL1" s="80"/>
+      <c r="FM1" s="80"/>
+      <c r="FN1" s="80"/>
+      <c r="FO1" s="80"/>
+      <c r="FP1" s="80"/>
+      <c r="FQ1" s="80"/>
+      <c r="FR1" s="80"/>
+      <c r="FS1" s="80"/>
+      <c r="FT1" s="80"/>
+      <c r="FU1" s="80"/>
+      <c r="FV1" s="80"/>
+      <c r="FW1" s="80"/>
+      <c r="FX1" s="80"/>
+      <c r="FY1" s="80"/>
+      <c r="FZ1" s="80"/>
+      <c r="GA1" s="80"/>
+      <c r="GB1" s="80"/>
+      <c r="GC1" s="80"/>
+      <c r="GD1" s="80"/>
+      <c r="GE1" s="80"/>
+      <c r="GF1" s="80"/>
+      <c r="GG1" s="80"/>
+      <c r="GH1" s="80"/>
+      <c r="GI1" s="80"/>
+      <c r="GJ1" s="80"/>
+      <c r="GK1" s="80"/>
+      <c r="GL1" s="80"/>
+      <c r="GM1" s="80"/>
+      <c r="GN1" s="80"/>
+      <c r="GO1" s="80"/>
+      <c r="GP1" s="80"/>
+      <c r="GQ1" s="80"/>
+      <c r="GR1" s="80"/>
+      <c r="GS1" s="80"/>
+      <c r="GT1" s="80"/>
+      <c r="GU1" s="80"/>
+      <c r="GV1" s="80"/>
+      <c r="GW1" s="80"/>
+      <c r="GX1" s="80"/>
+      <c r="GY1" s="80"/>
+      <c r="GZ1" s="80"/>
+      <c r="HA1" s="80"/>
+      <c r="HB1" s="80"/>
+      <c r="HC1" s="80"/>
+      <c r="HD1" s="80"/>
+      <c r="HE1" s="80"/>
+      <c r="HF1" s="80"/>
+      <c r="HG1" s="80"/>
+      <c r="HH1" s="80"/>
+      <c r="HI1" s="80"/>
+      <c r="HJ1" s="80"/>
+      <c r="HK1" s="80"/>
+      <c r="HL1" s="80"/>
+      <c r="HM1" s="80"/>
+      <c r="HN1" s="80"/>
+      <c r="HO1" s="80"/>
+      <c r="HP1" s="80"/>
+      <c r="HQ1" s="80"/>
+      <c r="HR1" s="80"/>
+      <c r="HS1" s="80"/>
+      <c r="HT1" s="80"/>
+      <c r="HU1" s="80"/>
+      <c r="HV1" s="80"/>
+      <c r="HW1" s="80"/>
+      <c r="HX1" s="80"/>
+      <c r="HY1" s="80"/>
+      <c r="HZ1" s="80"/>
+      <c r="IA1" s="80"/>
+      <c r="IB1" s="80"/>
+      <c r="IC1" s="80"/>
+      <c r="ID1" s="80"/>
+      <c r="IE1" s="80"/>
+      <c r="IF1" s="80"/>
+      <c r="IG1" s="80"/>
+      <c r="IH1" s="80"/>
+      <c r="II1" s="80"/>
+      <c r="IJ1" s="80"/>
+      <c r="IK1" s="80"/>
+      <c r="IL1" s="80"/>
+      <c r="IM1" s="80"/>
+      <c r="IN1" s="80"/>
+      <c r="IO1" s="80"/>
+      <c r="IP1" s="80"/>
+      <c r="IQ1" s="80"/>
+      <c r="IR1" s="80"/>
+      <c r="IS1" s="80"/>
+      <c r="IT1" s="80"/>
+      <c r="IU1" s="80"/>
     </row>
     <row r="2" spans="1:255" ht="17.100000000000001" customHeight="1">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="107"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="84">
+      <c r="D2" s="101"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78">
         <v>3</v>
       </c>
-      <c r="G2" s="83"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="95">
+      <c r="G2" s="77"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="89">
         <v>1</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
     </row>
     <row r="3" spans="1:255" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="16" t="s">
@@ -2937,10 +2940,10 @@
       <c r="B3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="97"/>
+      <c r="D3" s="91"/>
       <c r="E3" s="15">
         <v>1</v>
       </c>
@@ -2948,12 +2951,12 @@
       <c r="G3" s="15">
         <v>1</v>
       </c>
-      <c r="H3" s="90"/>
-      <c r="I3" s="97"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="91"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="96">
+      <c r="L3" s="84"/>
+      <c r="M3" s="90">
         <v>1</v>
       </c>
       <c r="N3" s="14" t="s">
@@ -2970,10 +2973,10 @@
       <c r="B4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="97"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="15">
         <v>1</v>
       </c>
@@ -2983,12 +2986,12 @@
       <c r="G4" s="15">
         <v>1</v>
       </c>
-      <c r="H4" s="90"/>
-      <c r="I4" s="97"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="91"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="96">
+      <c r="L4" s="84"/>
+      <c r="M4" s="90">
         <v>2</v>
       </c>
       <c r="N4" s="14" t="s">
@@ -3005,10 +3008,10 @@
       <c r="B5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="96">
+      <c r="D5" s="90">
         <v>3</v>
       </c>
       <c r="E5" s="8"/>
@@ -3016,12 +3019,12 @@
         <v>1</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="97"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="91"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="96">
+      <c r="L5" s="84"/>
+      <c r="M5" s="90">
         <v>2</v>
       </c>
       <c r="N5" s="14" t="s">
@@ -3038,21 +3041,21 @@
       <c r="B6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="97"/>
+      <c r="D6" s="91"/>
       <c r="E6" s="8"/>
       <c r="F6" s="15">
         <v>3</v>
       </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="97"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="91"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="96">
+      <c r="L6" s="84"/>
+      <c r="M6" s="90">
         <v>1</v>
       </c>
       <c r="N6" s="14" t="s">
@@ -3073,10 +3076,10 @@
       <c r="B7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="105" t="s">
+      <c r="C7" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="97"/>
+      <c r="D7" s="91"/>
       <c r="E7" s="15">
         <v>2</v>
       </c>
@@ -3084,12 +3087,12 @@
         <v>1</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="97"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="91"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="96">
+      <c r="L7" s="84"/>
+      <c r="M7" s="90">
         <v>1</v>
       </c>
       <c r="N7" s="14" t="s">
@@ -3110,10 +3113,10 @@
       <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="96">
+      <c r="D8" s="90">
         <v>2</v>
       </c>
       <c r="E8" s="15">
@@ -3123,12 +3126,12 @@
         <v>1</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="97"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="91"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="96">
+      <c r="L8" s="84"/>
+      <c r="M8" s="90">
         <v>2</v>
       </c>
       <c r="N8" s="14" t="s">
@@ -3145,10 +3148,10 @@
       <c r="B9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="96">
+      <c r="D9" s="90">
         <v>2</v>
       </c>
       <c r="E9" s="15">
@@ -3156,12 +3159,12 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="97"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="91"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="96">
+      <c r="L9" s="84"/>
+      <c r="M9" s="90">
         <v>1</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -3178,21 +3181,21 @@
       <c r="B10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="96">
+      <c r="D10" s="90">
         <v>5</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="97"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="91"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="96">
+      <c r="L10" s="84"/>
+      <c r="M10" s="90">
         <v>1</v>
       </c>
       <c r="N10" s="14" t="s">
@@ -3209,10 +3212,10 @@
       <c r="B11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="96">
+      <c r="D11" s="90">
         <v>3</v>
       </c>
       <c r="E11" s="8"/>
@@ -3220,12 +3223,12 @@
         <v>2</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="97"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="91"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="96">
+      <c r="L11" s="84"/>
+      <c r="M11" s="90">
         <v>1</v>
       </c>
       <c r="N11" s="14" t="s">
@@ -3242,10 +3245,10 @@
       <c r="B12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="96">
+      <c r="D12" s="90">
         <v>2</v>
       </c>
       <c r="E12" s="8"/>
@@ -3253,12 +3256,12 @@
       <c r="G12" s="15">
         <v>1</v>
       </c>
-      <c r="H12" s="90"/>
-      <c r="I12" s="97"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="91"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="96">
+      <c r="L12" s="84"/>
+      <c r="M12" s="90">
         <v>1</v>
       </c>
       <c r="N12" s="14" t="s">
@@ -3279,10 +3282,10 @@
       <c r="B13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="97"/>
+      <c r="D13" s="91"/>
       <c r="E13" s="15">
         <v>2</v>
       </c>
@@ -3290,12 +3293,12 @@
       <c r="G13" s="15">
         <v>2</v>
       </c>
-      <c r="H13" s="90"/>
-      <c r="I13" s="97"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="91"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="97"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="91"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
@@ -3308,10 +3311,10 @@
       <c r="B14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="96">
+      <c r="D14" s="90">
         <v>2</v>
       </c>
       <c r="E14" s="8"/>
@@ -3319,12 +3322,12 @@
       <c r="G14" s="15">
         <v>1</v>
       </c>
-      <c r="H14" s="90"/>
-      <c r="I14" s="97"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="91"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="96">
+      <c r="L14" s="84"/>
+      <c r="M14" s="90">
         <v>1</v>
       </c>
       <c r="N14" s="14" t="s">
@@ -3345,10 +3348,10 @@
       <c r="B15" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="97"/>
+      <c r="D15" s="91"/>
       <c r="E15" s="15">
         <v>2</v>
       </c>
@@ -3358,12 +3361,12 @@
       <c r="G15" s="15">
         <v>1</v>
       </c>
-      <c r="H15" s="90"/>
-      <c r="I15" s="97"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="91"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="96">
+      <c r="L15" s="84"/>
+      <c r="M15" s="90">
         <v>1</v>
       </c>
       <c r="N15" s="14" t="s">
@@ -3380,10 +3383,10 @@
       <c r="B16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="105" t="s">
+      <c r="C16" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="97"/>
+      <c r="D16" s="91"/>
       <c r="E16" s="15">
         <v>1</v>
       </c>
@@ -3393,12 +3396,12 @@
       <c r="G16" s="15">
         <v>1</v>
       </c>
-      <c r="H16" s="90"/>
-      <c r="I16" s="97"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="91"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="96">
+      <c r="L16" s="84"/>
+      <c r="M16" s="90">
         <v>1</v>
       </c>
       <c r="N16" s="14" t="s">
@@ -3415,21 +3418,21 @@
       <c r="B17" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="97"/>
+      <c r="D17" s="91"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="15">
         <v>3</v>
       </c>
-      <c r="H17" s="90"/>
-      <c r="I17" s="97"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="91"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="90"/>
-      <c r="M17" s="96">
+      <c r="L17" s="84"/>
+      <c r="M17" s="90">
         <v>1</v>
       </c>
       <c r="N17" s="14" t="s">
@@ -3446,10 +3449,10 @@
       <c r="B18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="105" t="s">
+      <c r="C18" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="96">
+      <c r="D18" s="90">
         <v>3</v>
       </c>
       <c r="E18" s="15">
@@ -3457,12 +3460,12 @@
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="97"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="91"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="97"/>
+      <c r="L18" s="84"/>
+      <c r="M18" s="91"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3475,10 +3478,10 @@
       <c r="B19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="105" t="s">
+      <c r="C19" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="97"/>
+      <c r="D19" s="91"/>
       <c r="E19" s="8"/>
       <c r="F19" s="15">
         <v>3</v>
@@ -3486,12 +3489,12 @@
       <c r="G19" s="15">
         <v>1</v>
       </c>
-      <c r="H19" s="90"/>
-      <c r="I19" s="97"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="91"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="96">
+      <c r="L19" s="84"/>
+      <c r="M19" s="90">
         <v>1</v>
       </c>
       <c r="N19" s="14" t="s">
@@ -3508,10 +3511,10 @@
       <c r="B20" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="105" t="s">
+      <c r="C20" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="97"/>
+      <c r="D20" s="91"/>
       <c r="E20" s="15">
         <v>2</v>
       </c>
@@ -3519,26 +3522,20 @@
         <v>2</v>
       </c>
       <c r="G20" s="8"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="97"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="91"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="96">
+      <c r="L20" s="84"/>
+      <c r="M20" s="90">
         <v>1</v>
       </c>
       <c r="N20" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="P20" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="14" t="s">
-        <v>40</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="14"/>
     </row>
     <row r="21" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="16" t="s">
@@ -3547,10 +3544,10 @@
       <c r="B21" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="105" t="s">
+      <c r="C21" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="96">
+      <c r="D21" s="90">
         <v>4</v>
       </c>
       <c r="E21" s="15">
@@ -3558,12 +3555,12 @@
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="97"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="91"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="90"/>
-      <c r="M21" s="97"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="91"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
@@ -3576,10 +3573,10 @@
       <c r="B22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="105" t="s">
+      <c r="C22" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="96">
+      <c r="D22" s="90">
         <v>2</v>
       </c>
       <c r="E22" s="15">
@@ -3589,12 +3586,12 @@
         <v>1</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="97"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="91"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="96">
+      <c r="L22" s="84"/>
+      <c r="M22" s="90">
         <v>1</v>
       </c>
       <c r="N22" s="14" t="s">
@@ -3611,10 +3608,10 @@
       <c r="B23" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="105" t="s">
+      <c r="C23" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="96">
+      <c r="D23" s="90">
         <v>3</v>
       </c>
       <c r="E23" s="15">
@@ -3624,12 +3621,12 @@
         <v>2</v>
       </c>
       <c r="G23" s="8"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="97"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="91"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="90"/>
-      <c r="M23" s="97"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="91"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
@@ -3642,10 +3639,10 @@
       <c r="B24" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="105" t="s">
+      <c r="C24" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="96">
+      <c r="D24" s="90">
         <v>3</v>
       </c>
       <c r="E24" s="8"/>
@@ -3655,12 +3652,12 @@
       <c r="G24" s="15">
         <v>1</v>
       </c>
-      <c r="H24" s="90"/>
-      <c r="I24" s="97"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="91"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="96">
+      <c r="L24" s="84"/>
+      <c r="M24" s="90">
         <v>1</v>
       </c>
       <c r="N24" s="14" t="s">
@@ -3677,10 +3674,10 @@
       <c r="B25" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="105" t="s">
+      <c r="C25" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="96">
+      <c r="D25" s="90">
         <v>2</v>
       </c>
       <c r="E25" s="15">
@@ -3690,12 +3687,12 @@
       <c r="G25" s="15">
         <v>2</v>
       </c>
-      <c r="H25" s="90"/>
-      <c r="I25" s="97"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="91"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="97"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="91"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
@@ -3708,10 +3705,10 @@
       <c r="B26" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="105" t="s">
+      <c r="C26" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="96">
+      <c r="D26" s="90">
         <v>2</v>
       </c>
       <c r="E26" s="8"/>
@@ -3719,12 +3716,12 @@
       <c r="G26" s="15">
         <v>2</v>
       </c>
-      <c r="H26" s="90"/>
-      <c r="I26" s="97"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="91"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="90"/>
-      <c r="M26" s="96">
+      <c r="L26" s="84"/>
+      <c r="M26" s="90">
         <v>2</v>
       </c>
       <c r="N26" s="14" t="s">
@@ -3741,10 +3738,10 @@
       <c r="B27" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="105" t="s">
+      <c r="C27" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="97"/>
+      <c r="D27" s="91"/>
       <c r="E27" s="8"/>
       <c r="F27" s="15">
         <v>1</v>
@@ -3752,12 +3749,12 @@
       <c r="G27" s="15">
         <v>3</v>
       </c>
-      <c r="H27" s="90"/>
-      <c r="I27" s="97"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="91"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="97"/>
+      <c r="L27" s="84"/>
+      <c r="M27" s="91"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
@@ -3770,21 +3767,21 @@
       <c r="B28" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="105" t="s">
+      <c r="C28" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="96">
+      <c r="D28" s="90">
         <v>5</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="97"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="91"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="96">
+      <c r="L28" s="84"/>
+      <c r="M28" s="90">
         <v>2</v>
       </c>
       <c r="N28" s="14" t="s">
@@ -3801,10 +3798,10 @@
       <c r="B29" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="105" t="s">
+      <c r="C29" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="96">
+      <c r="D29" s="90">
         <v>2</v>
       </c>
       <c r="E29" s="15">
@@ -3812,12 +3809,12 @@
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="97"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="91"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="96">
+      <c r="L29" s="84"/>
+      <c r="M29" s="90">
         <v>1</v>
       </c>
       <c r="N29" s="14" t="s">
@@ -3834,10 +3831,10 @@
       <c r="B30" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="105" t="s">
+      <c r="C30" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="97"/>
+      <c r="D30" s="91"/>
       <c r="E30" s="15">
         <v>2</v>
       </c>
@@ -3845,12 +3842,12 @@
         <v>2</v>
       </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="90"/>
-      <c r="I30" s="97"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="91"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="96">
+      <c r="L30" s="84"/>
+      <c r="M30" s="90">
         <v>1</v>
       </c>
       <c r="N30" s="14" t="s">
@@ -3867,10 +3864,10 @@
       <c r="B31" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="105" t="s">
+      <c r="C31" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="96">
+      <c r="D31" s="90">
         <v>1</v>
       </c>
       <c r="E31" s="8"/>
@@ -3880,12 +3877,12 @@
       <c r="G31" s="15">
         <v>1</v>
       </c>
-      <c r="H31" s="90"/>
-      <c r="I31" s="97"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="91"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="90"/>
-      <c r="M31" s="96">
+      <c r="L31" s="84"/>
+      <c r="M31" s="90">
         <v>2</v>
       </c>
       <c r="N31" s="14" t="s">
@@ -3902,10 +3899,10 @@
       <c r="B32" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="105" t="s">
+      <c r="C32" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="96">
+      <c r="D32" s="90">
         <v>3</v>
       </c>
       <c r="E32" s="8"/>
@@ -3913,12 +3910,12 @@
         <v>2</v>
       </c>
       <c r="G32" s="8"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="97"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="91"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="90"/>
-      <c r="M32" s="96">
+      <c r="L32" s="84"/>
+      <c r="M32" s="90">
         <v>1</v>
       </c>
       <c r="N32" s="14" t="s">
@@ -3935,10 +3932,10 @@
       <c r="B33" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="105" t="s">
+      <c r="C33" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="97"/>
+      <c r="D33" s="91"/>
       <c r="E33" s="15">
         <v>2</v>
       </c>
@@ -3946,12 +3943,12 @@
         <v>2</v>
       </c>
       <c r="G33" s="8"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="97"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="91"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="90"/>
-      <c r="M33" s="96">
+      <c r="L33" s="84"/>
+      <c r="M33" s="90">
         <v>1</v>
       </c>
       <c r="N33" s="14" t="s">
@@ -3968,10 +3965,10 @@
       <c r="B34" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="105" t="s">
+      <c r="C34" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="96">
+      <c r="D34" s="90">
         <v>3</v>
       </c>
       <c r="E34" s="15">
@@ -3981,12 +3978,12 @@
       <c r="G34" s="15">
         <v>1</v>
       </c>
-      <c r="H34" s="90"/>
-      <c r="I34" s="97"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="91"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="97"/>
+      <c r="L34" s="84"/>
+      <c r="M34" s="91"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
@@ -3999,10 +3996,10 @@
       <c r="B35" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="105" t="s">
+      <c r="C35" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="96">
+      <c r="D35" s="90">
         <v>2</v>
       </c>
       <c r="E35" s="8"/>
@@ -4012,12 +4009,12 @@
       <c r="G35" s="15">
         <v>2</v>
       </c>
-      <c r="H35" s="90"/>
-      <c r="I35" s="97"/>
+      <c r="H35" s="84"/>
+      <c r="I35" s="91"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="97"/>
+      <c r="L35" s="84"/>
+      <c r="M35" s="91"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -4030,10 +4027,10 @@
       <c r="B36" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="105" t="s">
+      <c r="C36" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="97"/>
+      <c r="D36" s="91"/>
       <c r="E36" s="8"/>
       <c r="F36" s="15">
         <v>2</v>
@@ -4041,12 +4038,12 @@
       <c r="G36" s="15">
         <v>1</v>
       </c>
-      <c r="H36" s="90"/>
-      <c r="I36" s="97"/>
+      <c r="H36" s="84"/>
+      <c r="I36" s="91"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="90"/>
-      <c r="M36" s="96">
+      <c r="L36" s="84"/>
+      <c r="M36" s="90">
         <v>1</v>
       </c>
       <c r="N36" s="14" t="s">
@@ -4067,10 +4064,10 @@
       <c r="B37" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="105" t="s">
+      <c r="C37" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="97"/>
+      <c r="D37" s="91"/>
       <c r="E37" s="15">
         <v>2</v>
       </c>
@@ -4078,12 +4075,12 @@
       <c r="G37" s="15">
         <v>1</v>
       </c>
-      <c r="H37" s="90"/>
-      <c r="I37" s="97"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="91"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="96">
+      <c r="L37" s="84"/>
+      <c r="M37" s="90">
         <v>1</v>
       </c>
       <c r="N37" s="14" t="s">
@@ -4104,10 +4101,10 @@
       <c r="B38" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="105" t="s">
+      <c r="C38" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="97"/>
+      <c r="D38" s="91"/>
       <c r="E38" s="15">
         <v>2</v>
       </c>
@@ -4115,14 +4112,14 @@
       <c r="G38" s="15">
         <v>1</v>
       </c>
-      <c r="H38" s="111">
-        <v>1</v>
-      </c>
-      <c r="I38" s="97"/>
+      <c r="H38" s="105">
+        <v>1</v>
+      </c>
+      <c r="I38" s="91"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="96">
+      <c r="L38" s="84"/>
+      <c r="M38" s="90">
         <v>2</v>
       </c>
       <c r="N38" s="14" t="s">
@@ -4133,7 +4130,7 @@
         <v>2</v>
       </c>
       <c r="Q38" s="14" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="17.100000000000001" customHeight="1">
@@ -4143,10 +4140,10 @@
       <c r="B39" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="105" t="s">
+      <c r="C39" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="96">
+      <c r="D39" s="90">
         <v>2</v>
       </c>
       <c r="E39" s="8"/>
@@ -4154,14 +4151,14 @@
       <c r="G39" s="15">
         <v>1</v>
       </c>
-      <c r="H39" s="111">
-        <v>1</v>
-      </c>
-      <c r="I39" s="97"/>
+      <c r="H39" s="105">
+        <v>1</v>
+      </c>
+      <c r="I39" s="91"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
-      <c r="L39" s="90"/>
-      <c r="M39" s="96">
+      <c r="L39" s="84"/>
+      <c r="M39" s="90">
         <v>3</v>
       </c>
       <c r="N39" s="14" t="s">
@@ -4182,21 +4179,21 @@
       <c r="B40" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="105" t="s">
+      <c r="C40" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="97"/>
+      <c r="D40" s="91"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="111">
+      <c r="H40" s="105">
         <v>3</v>
       </c>
-      <c r="I40" s="97"/>
+      <c r="I40" s="91"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="90"/>
-      <c r="M40" s="96">
+      <c r="L40" s="84"/>
+      <c r="M40" s="90">
         <v>2</v>
       </c>
       <c r="N40" s="14" t="s">
@@ -4217,10 +4214,10 @@
       <c r="B41" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="105" t="s">
+      <c r="C41" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="96">
+      <c r="D41" s="90">
         <v>2</v>
       </c>
       <c r="E41" s="8"/>
@@ -4228,14 +4225,14 @@
         <v>2</v>
       </c>
       <c r="G41" s="8"/>
-      <c r="H41" s="111">
-        <v>1</v>
-      </c>
-      <c r="I41" s="97"/>
+      <c r="H41" s="105">
+        <v>1</v>
+      </c>
+      <c r="I41" s="91"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="96">
+      <c r="L41" s="84"/>
+      <c r="M41" s="90">
         <v>1</v>
       </c>
       <c r="N41" s="14" t="s">
@@ -4254,10 +4251,10 @@
       <c r="B42" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="105" t="s">
+      <c r="C42" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="96">
+      <c r="D42" s="90">
         <v>2</v>
       </c>
       <c r="E42" s="15">
@@ -4267,12 +4264,12 @@
         <v>2</v>
       </c>
       <c r="G42" s="8"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="97"/>
+      <c r="H42" s="84"/>
+      <c r="I42" s="91"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
-      <c r="L42" s="90"/>
-      <c r="M42" s="96">
+      <c r="L42" s="84"/>
+      <c r="M42" s="90">
         <v>1</v>
       </c>
       <c r="N42" s="14" t="s">
@@ -4291,10 +4288,10 @@
       <c r="B43" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="105" t="s">
+      <c r="C43" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="97"/>
+      <c r="D43" s="91"/>
       <c r="E43" s="8"/>
       <c r="F43" s="15">
         <v>1</v>
@@ -4302,14 +4299,14 @@
       <c r="G43" s="15">
         <v>1</v>
       </c>
-      <c r="H43" s="111">
-        <v>1</v>
-      </c>
-      <c r="I43" s="97"/>
+      <c r="H43" s="105">
+        <v>1</v>
+      </c>
+      <c r="I43" s="91"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="96">
+      <c r="L43" s="84"/>
+      <c r="M43" s="90">
         <v>3</v>
       </c>
       <c r="N43" s="14" t="s">
@@ -4326,10 +4323,10 @@
       <c r="B44" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="105" t="s">
+      <c r="C44" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="97"/>
+      <c r="D44" s="91"/>
       <c r="E44" s="15">
         <v>1</v>
       </c>
@@ -4337,14 +4334,14 @@
       <c r="G44" s="15">
         <v>1</v>
       </c>
-      <c r="H44" s="111">
-        <v>1</v>
-      </c>
-      <c r="I44" s="97"/>
+      <c r="H44" s="105">
+        <v>1</v>
+      </c>
+      <c r="I44" s="91"/>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
-      <c r="L44" s="90"/>
-      <c r="M44" s="96">
+      <c r="L44" s="84"/>
+      <c r="M44" s="90">
         <v>3</v>
       </c>
       <c r="N44" s="6" t="s">
@@ -4361,23 +4358,23 @@
       <c r="B45" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C45" s="105" t="s">
+      <c r="C45" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="96">
+      <c r="D45" s="90">
         <v>4</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="111">
-        <v>1</v>
-      </c>
-      <c r="I45" s="97"/>
+      <c r="H45" s="105">
+        <v>1</v>
+      </c>
+      <c r="I45" s="91"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
-      <c r="L45" s="90"/>
-      <c r="M45" s="96">
+      <c r="L45" s="84"/>
+      <c r="M45" s="90">
         <v>3</v>
       </c>
       <c r="N45" s="14" t="s">
@@ -4394,21 +4391,21 @@
       <c r="B46" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="105" t="s">
+      <c r="C46" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="96">
+      <c r="D46" s="90">
         <v>4</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="97"/>
+      <c r="H46" s="84"/>
+      <c r="I46" s="91"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
-      <c r="L46" s="90"/>
-      <c r="M46" s="96">
+      <c r="L46" s="84"/>
+      <c r="M46" s="90">
         <v>2</v>
       </c>
       <c r="N46" s="14" t="s">
@@ -4425,10 +4422,10 @@
       <c r="B47" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="105" t="s">
+      <c r="C47" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="96">
+      <c r="D47" s="90">
         <v>2</v>
       </c>
       <c r="E47" s="8"/>
@@ -4436,12 +4433,12 @@
         <v>2</v>
       </c>
       <c r="G47" s="8"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="97"/>
+      <c r="H47" s="84"/>
+      <c r="I47" s="91"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
-      <c r="L47" s="90"/>
-      <c r="M47" s="96">
+      <c r="L47" s="84"/>
+      <c r="M47" s="90">
         <v>2</v>
       </c>
       <c r="N47" s="14" t="s">
@@ -4462,10 +4459,10 @@
       <c r="B48" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="105" t="s">
+      <c r="C48" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="96">
+      <c r="D48" s="90">
         <v>12</v>
       </c>
       <c r="E48" s="8"/>
@@ -4473,14 +4470,14 @@
         <v>10</v>
       </c>
       <c r="G48" s="8"/>
-      <c r="H48" s="111">
+      <c r="H48" s="105">
         <v>6</v>
       </c>
-      <c r="I48" s="97"/>
+      <c r="I48" s="91"/>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
-      <c r="L48" s="90"/>
-      <c r="M48" s="97"/>
+      <c r="L48" s="84"/>
+      <c r="M48" s="91"/>
       <c r="N48" s="14" t="s">
         <v>74</v>
       </c>
@@ -4495,10 +4492,10 @@
       <c r="B49" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="105" t="s">
+      <c r="C49" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="97"/>
+      <c r="D49" s="91"/>
       <c r="E49" s="15">
         <v>10</v>
       </c>
@@ -4506,14 +4503,14 @@
         <v>10</v>
       </c>
       <c r="G49" s="8"/>
-      <c r="H49" s="111">
+      <c r="H49" s="105">
         <v>6</v>
       </c>
-      <c r="I49" s="97"/>
+      <c r="I49" s="91"/>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
-      <c r="L49" s="90"/>
-      <c r="M49" s="97"/>
+      <c r="L49" s="84"/>
+      <c r="M49" s="91"/>
       <c r="N49" s="14" t="s">
         <v>74</v>
       </c>
@@ -4528,10 +4525,10 @@
       <c r="B50" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="105" t="s">
+      <c r="C50" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="96">
+      <c r="D50" s="90">
         <v>12</v>
       </c>
       <c r="E50" s="15">
@@ -4539,14 +4536,14 @@
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="111">
+      <c r="H50" s="105">
         <v>6</v>
       </c>
-      <c r="I50" s="97"/>
+      <c r="I50" s="91"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
-      <c r="L50" s="90"/>
-      <c r="M50" s="97"/>
+      <c r="L50" s="84"/>
+      <c r="M50" s="91"/>
       <c r="N50" s="14" t="s">
         <v>74</v>
       </c>
@@ -4561,10 +4558,10 @@
       <c r="B51" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="105" t="s">
+      <c r="C51" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="97"/>
+      <c r="D51" s="91"/>
       <c r="E51" s="8"/>
       <c r="F51" s="15">
         <v>10</v>
@@ -4572,14 +4569,14 @@
       <c r="G51" s="15">
         <v>8</v>
       </c>
-      <c r="H51" s="111">
+      <c r="H51" s="105">
         <v>6</v>
       </c>
-      <c r="I51" s="97"/>
+      <c r="I51" s="91"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
-      <c r="L51" s="90"/>
-      <c r="M51" s="97"/>
+      <c r="L51" s="84"/>
+      <c r="M51" s="91"/>
       <c r="N51" s="14" t="s">
         <v>74</v>
       </c>
@@ -4594,10 +4591,10 @@
       <c r="B52" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="105" t="s">
+      <c r="C52" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="97"/>
+      <c r="D52" s="91"/>
       <c r="E52" s="15">
         <v>10</v>
       </c>
@@ -4605,14 +4602,14 @@
       <c r="G52" s="15">
         <v>8</v>
       </c>
-      <c r="H52" s="111">
+      <c r="H52" s="105">
         <v>6</v>
       </c>
-      <c r="I52" s="97"/>
+      <c r="I52" s="91"/>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
-      <c r="L52" s="90"/>
-      <c r="M52" s="97"/>
+      <c r="L52" s="84"/>
+      <c r="M52" s="91"/>
       <c r="N52" s="14" t="s">
         <v>74</v>
       </c>
@@ -4627,10 +4624,10 @@
       <c r="B53" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="105" t="s">
+      <c r="C53" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="96">
+      <c r="D53" s="90">
         <v>2</v>
       </c>
       <c r="E53" s="8"/>
@@ -4638,12 +4635,12 @@
       <c r="G53" s="15">
         <v>2</v>
       </c>
-      <c r="H53" s="90"/>
-      <c r="I53" s="97"/>
+      <c r="H53" s="84"/>
+      <c r="I53" s="91"/>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
-      <c r="L53" s="90"/>
-      <c r="M53" s="96">
+      <c r="L53" s="84"/>
+      <c r="M53" s="90">
         <v>2</v>
       </c>
       <c r="N53" s="14" t="s">
@@ -4664,21 +4661,21 @@
       <c r="B54" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="105" t="s">
+      <c r="C54" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D54" s="97"/>
+      <c r="D54" s="91"/>
       <c r="E54" s="8"/>
       <c r="F54" s="15">
         <v>3</v>
       </c>
       <c r="G54" s="8"/>
-      <c r="H54" s="90"/>
-      <c r="I54" s="97"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="91"/>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
-      <c r="L54" s="90"/>
-      <c r="M54" s="96">
+      <c r="L54" s="84"/>
+      <c r="M54" s="90">
         <v>1</v>
       </c>
       <c r="N54" s="14" t="s">
@@ -4699,21 +4696,21 @@
       <c r="B55" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="105" t="s">
+      <c r="C55" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D55" s="97"/>
+      <c r="D55" s="91"/>
       <c r="E55" s="15">
         <v>3</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="90"/>
-      <c r="I55" s="97"/>
+      <c r="H55" s="84"/>
+      <c r="I55" s="91"/>
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
-      <c r="L55" s="90"/>
-      <c r="M55" s="96">
+      <c r="L55" s="84"/>
+      <c r="M55" s="90">
         <v>1</v>
       </c>
       <c r="N55" s="14" t="s">
@@ -4734,10 +4731,10 @@
       <c r="B56" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="105" t="s">
+      <c r="C56" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D56" s="96">
+      <c r="D56" s="90">
         <v>2</v>
       </c>
       <c r="E56" s="15">
@@ -4747,14 +4744,14 @@
         <v>2</v>
       </c>
       <c r="G56" s="8"/>
-      <c r="H56" s="111">
-        <v>2</v>
-      </c>
-      <c r="I56" s="97"/>
+      <c r="H56" s="105">
+        <v>2</v>
+      </c>
+      <c r="I56" s="91"/>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
-      <c r="L56" s="90"/>
-      <c r="M56" s="96">
+      <c r="L56" s="84"/>
+      <c r="M56" s="90">
         <v>1</v>
       </c>
       <c r="N56" s="14" t="s">
@@ -4775,21 +4772,21 @@
       <c r="B57" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C57" s="105" t="s">
+      <c r="C57" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D57" s="97"/>
+      <c r="D57" s="91"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="15">
         <v>3</v>
       </c>
-      <c r="H57" s="90"/>
-      <c r="I57" s="97"/>
+      <c r="H57" s="84"/>
+      <c r="I57" s="91"/>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
-      <c r="L57" s="90"/>
-      <c r="M57" s="96">
+      <c r="L57" s="84"/>
+      <c r="M57" s="90">
         <v>2</v>
       </c>
       <c r="N57" s="14" t="s">
@@ -4806,10 +4803,10 @@
       <c r="B58" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C58" s="105" t="s">
+      <c r="C58" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D58" s="97"/>
+      <c r="D58" s="91"/>
       <c r="E58" s="15">
         <v>2</v>
       </c>
@@ -4817,12 +4814,12 @@
         <v>2</v>
       </c>
       <c r="G58" s="8"/>
-      <c r="H58" s="90"/>
-      <c r="I58" s="97"/>
+      <c r="H58" s="84"/>
+      <c r="I58" s="91"/>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
-      <c r="L58" s="90"/>
-      <c r="M58" s="96">
+      <c r="L58" s="84"/>
+      <c r="M58" s="90">
         <v>1</v>
       </c>
       <c r="N58" s="14" t="s">
@@ -4843,19 +4840,19 @@
       <c r="B59" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="105" t="s">
+      <c r="C59" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="97"/>
+      <c r="D59" s="91"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="90"/>
-      <c r="I59" s="97"/>
+      <c r="H59" s="84"/>
+      <c r="I59" s="91"/>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
-      <c r="L59" s="90"/>
-      <c r="M59" s="96">
+      <c r="L59" s="84"/>
+      <c r="M59" s="90">
         <v>2</v>
       </c>
       <c r="N59" s="14" t="s">
@@ -4876,15 +4873,15 @@
       <c r="B60" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C60" s="105" t="s">
+      <c r="C60" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D60" s="97"/>
+      <c r="D60" s="91"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="90"/>
-      <c r="I60" s="96">
+      <c r="H60" s="84"/>
+      <c r="I60" s="90">
         <v>1</v>
       </c>
       <c r="J60" s="6" t="s">
@@ -4893,10 +4890,10 @@
       <c r="K60" s="15">
         <v>1</v>
       </c>
-      <c r="L60" s="91" t="s">
+      <c r="L60" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="M60" s="96">
+      <c r="M60" s="90">
         <v>1</v>
       </c>
       <c r="N60" s="14" t="s">
@@ -4917,23 +4914,23 @@
       <c r="B61" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="105" t="s">
+      <c r="C61" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="97"/>
+      <c r="D61" s="91"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="90"/>
-      <c r="I61" s="96">
+      <c r="H61" s="84"/>
+      <c r="I61" s="90">
         <v>2</v>
       </c>
       <c r="J61" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K61" s="21"/>
-      <c r="L61" s="90"/>
-      <c r="M61" s="96">
+      <c r="L61" s="84"/>
+      <c r="M61" s="90">
         <v>1</v>
       </c>
       <c r="N61" s="14" t="s">
@@ -4954,19 +4951,19 @@
       <c r="B62" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C62" s="105" t="s">
+      <c r="C62" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D62" s="97"/>
+      <c r="D62" s="91"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="90"/>
-      <c r="I62" s="97"/>
+      <c r="H62" s="84"/>
+      <c r="I62" s="91"/>
       <c r="J62" s="8"/>
       <c r="K62" s="21"/>
-      <c r="L62" s="90"/>
-      <c r="M62" s="96">
+      <c r="L62" s="84"/>
+      <c r="M62" s="90">
         <v>1</v>
       </c>
       <c r="N62" s="14" t="s">
@@ -4983,23 +4980,23 @@
       <c r="B63" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="105" t="s">
+      <c r="C63" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="97"/>
+      <c r="D63" s="91"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="90"/>
-      <c r="I63" s="96">
+      <c r="H63" s="84"/>
+      <c r="I63" s="90">
         <v>2</v>
       </c>
       <c r="J63" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K63" s="21"/>
-      <c r="L63" s="90"/>
-      <c r="M63" s="96">
+      <c r="L63" s="84"/>
+      <c r="M63" s="90">
         <v>1</v>
       </c>
       <c r="N63" s="14" t="s">
@@ -5020,19 +5017,19 @@
       <c r="B64" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="105" t="s">
+      <c r="C64" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="97"/>
+      <c r="D64" s="91"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="90"/>
-      <c r="I64" s="97"/>
+      <c r="H64" s="84"/>
+      <c r="I64" s="91"/>
       <c r="J64" s="8"/>
       <c r="K64" s="21"/>
-      <c r="L64" s="90"/>
-      <c r="M64" s="96">
+      <c r="L64" s="84"/>
+      <c r="M64" s="90">
         <v>1</v>
       </c>
       <c r="N64" s="14" t="s">
@@ -5049,23 +5046,23 @@
       <c r="B65" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="105" t="s">
+      <c r="C65" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="97"/>
+      <c r="D65" s="91"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="90"/>
-      <c r="I65" s="96">
+      <c r="H65" s="84"/>
+      <c r="I65" s="90">
         <v>3</v>
       </c>
       <c r="J65" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K65" s="21"/>
-      <c r="L65" s="90"/>
-      <c r="M65" s="96">
+      <c r="L65" s="84"/>
+      <c r="M65" s="90">
         <v>1</v>
       </c>
       <c r="N65" s="14" t="s">
@@ -5086,23 +5083,23 @@
       <c r="B66" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="105" t="s">
+      <c r="C66" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="97"/>
+      <c r="D66" s="91"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
-      <c r="H66" s="90"/>
-      <c r="I66" s="96">
+      <c r="H66" s="84"/>
+      <c r="I66" s="90">
         <v>1</v>
       </c>
       <c r="J66" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K66" s="21"/>
-      <c r="L66" s="90"/>
-      <c r="M66" s="96">
+      <c r="L66" s="84"/>
+      <c r="M66" s="90">
         <v>1</v>
       </c>
       <c r="N66" s="6" t="s">
@@ -5125,23 +5122,23 @@
       <c r="B67" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="105" t="s">
+      <c r="C67" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="97"/>
+      <c r="D67" s="91"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="90"/>
-      <c r="I67" s="96">
+      <c r="H67" s="84"/>
+      <c r="I67" s="90">
         <v>2</v>
       </c>
       <c r="J67" s="6" t="s">
         <v>5</v>
       </c>
       <c r="K67" s="21"/>
-      <c r="L67" s="90"/>
-      <c r="M67" s="96">
+      <c r="L67" s="84"/>
+      <c r="M67" s="90">
         <v>1</v>
       </c>
       <c r="N67" s="14" t="s">
@@ -5162,23 +5159,23 @@
       <c r="B68" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C68" s="105" t="s">
+      <c r="C68" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D68" s="97"/>
+      <c r="D68" s="91"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
-      <c r="H68" s="90"/>
-      <c r="I68" s="96">
+      <c r="H68" s="84"/>
+      <c r="I68" s="90">
         <v>2</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>7</v>
       </c>
       <c r="K68" s="21"/>
-      <c r="L68" s="90"/>
-      <c r="M68" s="96">
+      <c r="L68" s="84"/>
+      <c r="M68" s="90">
         <v>1</v>
       </c>
       <c r="N68" s="14" t="s">
@@ -5199,15 +5196,15 @@
       <c r="B69" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C69" s="105" t="s">
+      <c r="C69" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D69" s="97"/>
+      <c r="D69" s="91"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="90"/>
-      <c r="I69" s="96">
+      <c r="H69" s="84"/>
+      <c r="I69" s="90">
         <v>1</v>
       </c>
       <c r="J69" s="6" t="s">
@@ -5216,10 +5213,10 @@
       <c r="K69" s="15">
         <v>2</v>
       </c>
-      <c r="L69" s="91" t="s">
+      <c r="L69" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="M69" s="96">
+      <c r="M69" s="90">
         <v>1</v>
       </c>
       <c r="N69" s="14" t="s">
@@ -5240,19 +5237,19 @@
       <c r="B70" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="105" t="s">
+      <c r="C70" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="108"/>
+      <c r="D70" s="102"/>
       <c r="E70" s="21"/>
       <c r="F70" s="21"/>
       <c r="G70" s="21"/>
-      <c r="H70" s="93"/>
-      <c r="I70" s="108"/>
+      <c r="H70" s="87"/>
+      <c r="I70" s="102"/>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
-      <c r="L70" s="90"/>
-      <c r="M70" s="96">
+      <c r="L70" s="84"/>
+      <c r="M70" s="90">
         <v>1</v>
       </c>
       <c r="N70" s="14" t="s">
@@ -5269,23 +5266,23 @@
       <c r="B71" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C71" s="105" t="s">
+      <c r="C71" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D71" s="108"/>
+      <c r="D71" s="102"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="90"/>
-      <c r="I71" s="96">
+      <c r="H71" s="84"/>
+      <c r="I71" s="90">
         <v>1</v>
       </c>
       <c r="J71" s="14" t="s">
         <v>6</v>
       </c>
       <c r="K71" s="24"/>
-      <c r="L71" s="92"/>
-      <c r="M71" s="96">
+      <c r="L71" s="86"/>
+      <c r="M71" s="90">
         <v>1</v>
       </c>
       <c r="N71" s="14" t="s">
@@ -5308,23 +5305,23 @@
       <c r="B72" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C72" s="105" t="s">
+      <c r="C72" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D72" s="108"/>
+      <c r="D72" s="102"/>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="90"/>
-      <c r="I72" s="96">
+      <c r="H72" s="84"/>
+      <c r="I72" s="90">
         <v>2</v>
       </c>
       <c r="J72" s="14" t="s">
         <v>4</v>
       </c>
       <c r="K72" s="24"/>
-      <c r="L72" s="92"/>
-      <c r="M72" s="96">
+      <c r="L72" s="86"/>
+      <c r="M72" s="90">
         <v>1</v>
       </c>
       <c r="N72" s="14" t="s">
@@ -5338,30 +5335,30 @@
       </c>
       <c r="Q72" s="25"/>
     </row>
-    <row r="73" spans="1:255" s="102" customFormat="1" ht="15.75" customHeight="1">
+    <row r="73" spans="1:255" s="96" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B73" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="106" t="s">
+      <c r="C73" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="D73" s="109"/>
+      <c r="D73" s="103"/>
       <c r="E73" s="29"/>
       <c r="F73" s="29"/>
       <c r="G73" s="29"/>
-      <c r="H73" s="112"/>
-      <c r="I73" s="98">
+      <c r="H73" s="106"/>
+      <c r="I73" s="92">
         <v>1</v>
       </c>
       <c r="J73" s="32" t="s">
         <v>7</v>
       </c>
       <c r="K73" s="29"/>
-      <c r="L73" s="100"/>
-      <c r="M73" s="98">
+      <c r="L73" s="94"/>
+      <c r="M73" s="92">
         <v>1</v>
       </c>
       <c r="N73" s="32" t="s">
@@ -5374,244 +5371,244 @@
       <c r="Q73" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="R73" s="101"/>
-      <c r="S73" s="101"/>
-      <c r="T73" s="101"/>
-      <c r="U73" s="101"/>
-      <c r="V73" s="101"/>
-      <c r="W73" s="101"/>
-      <c r="X73" s="101"/>
-      <c r="Y73" s="101"/>
-      <c r="Z73" s="101"/>
-      <c r="AA73" s="101"/>
-      <c r="AB73" s="101"/>
-      <c r="AC73" s="101"/>
-      <c r="AD73" s="101"/>
-      <c r="AE73" s="101"/>
-      <c r="AF73" s="101"/>
-      <c r="AG73" s="101"/>
-      <c r="AH73" s="101"/>
-      <c r="AI73" s="101"/>
-      <c r="AJ73" s="101"/>
-      <c r="AK73" s="101"/>
-      <c r="AL73" s="101"/>
-      <c r="AM73" s="101"/>
-      <c r="AN73" s="101"/>
-      <c r="AO73" s="101"/>
-      <c r="AP73" s="101"/>
-      <c r="AQ73" s="101"/>
-      <c r="AR73" s="101"/>
-      <c r="AS73" s="101"/>
-      <c r="AT73" s="101"/>
-      <c r="AU73" s="101"/>
-      <c r="AV73" s="101"/>
-      <c r="AW73" s="101"/>
-      <c r="AX73" s="101"/>
-      <c r="AY73" s="101"/>
-      <c r="AZ73" s="101"/>
-      <c r="BA73" s="101"/>
-      <c r="BB73" s="101"/>
-      <c r="BC73" s="101"/>
-      <c r="BD73" s="101"/>
-      <c r="BE73" s="101"/>
-      <c r="BF73" s="101"/>
-      <c r="BG73" s="101"/>
-      <c r="BH73" s="101"/>
-      <c r="BI73" s="101"/>
-      <c r="BJ73" s="101"/>
-      <c r="BK73" s="101"/>
-      <c r="BL73" s="101"/>
-      <c r="BM73" s="101"/>
-      <c r="BN73" s="101"/>
-      <c r="BO73" s="101"/>
-      <c r="BP73" s="101"/>
-      <c r="BQ73" s="101"/>
-      <c r="BR73" s="101"/>
-      <c r="BS73" s="101"/>
-      <c r="BT73" s="101"/>
-      <c r="BU73" s="101"/>
-      <c r="BV73" s="101"/>
-      <c r="BW73" s="101"/>
-      <c r="BX73" s="101"/>
-      <c r="BY73" s="101"/>
-      <c r="BZ73" s="101"/>
-      <c r="CA73" s="101"/>
-      <c r="CB73" s="101"/>
-      <c r="CC73" s="101"/>
-      <c r="CD73" s="101"/>
-      <c r="CE73" s="101"/>
-      <c r="CF73" s="101"/>
-      <c r="CG73" s="101"/>
-      <c r="CH73" s="101"/>
-      <c r="CI73" s="101"/>
-      <c r="CJ73" s="101"/>
-      <c r="CK73" s="101"/>
-      <c r="CL73" s="101"/>
-      <c r="CM73" s="101"/>
-      <c r="CN73" s="101"/>
-      <c r="CO73" s="101"/>
-      <c r="CP73" s="101"/>
-      <c r="CQ73" s="101"/>
-      <c r="CR73" s="101"/>
-      <c r="CS73" s="101"/>
-      <c r="CT73" s="101"/>
-      <c r="CU73" s="101"/>
-      <c r="CV73" s="101"/>
-      <c r="CW73" s="101"/>
-      <c r="CX73" s="101"/>
-      <c r="CY73" s="101"/>
-      <c r="CZ73" s="101"/>
-      <c r="DA73" s="101"/>
-      <c r="DB73" s="101"/>
-      <c r="DC73" s="101"/>
-      <c r="DD73" s="101"/>
-      <c r="DE73" s="101"/>
-      <c r="DF73" s="101"/>
-      <c r="DG73" s="101"/>
-      <c r="DH73" s="101"/>
-      <c r="DI73" s="101"/>
-      <c r="DJ73" s="101"/>
-      <c r="DK73" s="101"/>
-      <c r="DL73" s="101"/>
-      <c r="DM73" s="101"/>
-      <c r="DN73" s="101"/>
-      <c r="DO73" s="101"/>
-      <c r="DP73" s="101"/>
-      <c r="DQ73" s="101"/>
-      <c r="DR73" s="101"/>
-      <c r="DS73" s="101"/>
-      <c r="DT73" s="101"/>
-      <c r="DU73" s="101"/>
-      <c r="DV73" s="101"/>
-      <c r="DW73" s="101"/>
-      <c r="DX73" s="101"/>
-      <c r="DY73" s="101"/>
-      <c r="DZ73" s="101"/>
-      <c r="EA73" s="101"/>
-      <c r="EB73" s="101"/>
-      <c r="EC73" s="101"/>
-      <c r="ED73" s="101"/>
-      <c r="EE73" s="101"/>
-      <c r="EF73" s="101"/>
-      <c r="EG73" s="101"/>
-      <c r="EH73" s="101"/>
-      <c r="EI73" s="101"/>
-      <c r="EJ73" s="101"/>
-      <c r="EK73" s="101"/>
-      <c r="EL73" s="101"/>
-      <c r="EM73" s="101"/>
-      <c r="EN73" s="101"/>
-      <c r="EO73" s="101"/>
-      <c r="EP73" s="101"/>
-      <c r="EQ73" s="101"/>
-      <c r="ER73" s="101"/>
-      <c r="ES73" s="101"/>
-      <c r="ET73" s="101"/>
-      <c r="EU73" s="101"/>
-      <c r="EV73" s="101"/>
-      <c r="EW73" s="101"/>
-      <c r="EX73" s="101"/>
-      <c r="EY73" s="101"/>
-      <c r="EZ73" s="101"/>
-      <c r="FA73" s="101"/>
-      <c r="FB73" s="101"/>
-      <c r="FC73" s="101"/>
-      <c r="FD73" s="101"/>
-      <c r="FE73" s="101"/>
-      <c r="FF73" s="101"/>
-      <c r="FG73" s="101"/>
-      <c r="FH73" s="101"/>
-      <c r="FI73" s="101"/>
-      <c r="FJ73" s="101"/>
-      <c r="FK73" s="101"/>
-      <c r="FL73" s="101"/>
-      <c r="FM73" s="101"/>
-      <c r="FN73" s="101"/>
-      <c r="FO73" s="101"/>
-      <c r="FP73" s="101"/>
-      <c r="FQ73" s="101"/>
-      <c r="FR73" s="101"/>
-      <c r="FS73" s="101"/>
-      <c r="FT73" s="101"/>
-      <c r="FU73" s="101"/>
-      <c r="FV73" s="101"/>
-      <c r="FW73" s="101"/>
-      <c r="FX73" s="101"/>
-      <c r="FY73" s="101"/>
-      <c r="FZ73" s="101"/>
-      <c r="GA73" s="101"/>
-      <c r="GB73" s="101"/>
-      <c r="GC73" s="101"/>
-      <c r="GD73" s="101"/>
-      <c r="GE73" s="101"/>
-      <c r="GF73" s="101"/>
-      <c r="GG73" s="101"/>
-      <c r="GH73" s="101"/>
-      <c r="GI73" s="101"/>
-      <c r="GJ73" s="101"/>
-      <c r="GK73" s="101"/>
-      <c r="GL73" s="101"/>
-      <c r="GM73" s="101"/>
-      <c r="GN73" s="101"/>
-      <c r="GO73" s="101"/>
-      <c r="GP73" s="101"/>
-      <c r="GQ73" s="101"/>
-      <c r="GR73" s="101"/>
-      <c r="GS73" s="101"/>
-      <c r="GT73" s="101"/>
-      <c r="GU73" s="101"/>
-      <c r="GV73" s="101"/>
-      <c r="GW73" s="101"/>
-      <c r="GX73" s="101"/>
-      <c r="GY73" s="101"/>
-      <c r="GZ73" s="101"/>
-      <c r="HA73" s="101"/>
-      <c r="HB73" s="101"/>
-      <c r="HC73" s="101"/>
-      <c r="HD73" s="101"/>
-      <c r="HE73" s="101"/>
-      <c r="HF73" s="101"/>
-      <c r="HG73" s="101"/>
-      <c r="HH73" s="101"/>
-      <c r="HI73" s="101"/>
-      <c r="HJ73" s="101"/>
-      <c r="HK73" s="101"/>
-      <c r="HL73" s="101"/>
-      <c r="HM73" s="101"/>
-      <c r="HN73" s="101"/>
-      <c r="HO73" s="101"/>
-      <c r="HP73" s="101"/>
-      <c r="HQ73" s="101"/>
-      <c r="HR73" s="101"/>
-      <c r="HS73" s="101"/>
-      <c r="HT73" s="101"/>
-      <c r="HU73" s="101"/>
-      <c r="HV73" s="101"/>
-      <c r="HW73" s="101"/>
-      <c r="HX73" s="101"/>
-      <c r="HY73" s="101"/>
-      <c r="HZ73" s="101"/>
-      <c r="IA73" s="101"/>
-      <c r="IB73" s="101"/>
-      <c r="IC73" s="101"/>
-      <c r="ID73" s="101"/>
-      <c r="IE73" s="101"/>
-      <c r="IF73" s="101"/>
-      <c r="IG73" s="101"/>
-      <c r="IH73" s="101"/>
-      <c r="II73" s="101"/>
-      <c r="IJ73" s="101"/>
-      <c r="IK73" s="101"/>
-      <c r="IL73" s="101"/>
-      <c r="IM73" s="101"/>
-      <c r="IN73" s="101"/>
-      <c r="IO73" s="101"/>
-      <c r="IP73" s="101"/>
-      <c r="IQ73" s="101"/>
-      <c r="IR73" s="101"/>
-      <c r="IS73" s="101"/>
-      <c r="IT73" s="101"/>
-      <c r="IU73" s="101"/>
+      <c r="R73" s="95"/>
+      <c r="S73" s="95"/>
+      <c r="T73" s="95"/>
+      <c r="U73" s="95"/>
+      <c r="V73" s="95"/>
+      <c r="W73" s="95"/>
+      <c r="X73" s="95"/>
+      <c r="Y73" s="95"/>
+      <c r="Z73" s="95"/>
+      <c r="AA73" s="95"/>
+      <c r="AB73" s="95"/>
+      <c r="AC73" s="95"/>
+      <c r="AD73" s="95"/>
+      <c r="AE73" s="95"/>
+      <c r="AF73" s="95"/>
+      <c r="AG73" s="95"/>
+      <c r="AH73" s="95"/>
+      <c r="AI73" s="95"/>
+      <c r="AJ73" s="95"/>
+      <c r="AK73" s="95"/>
+      <c r="AL73" s="95"/>
+      <c r="AM73" s="95"/>
+      <c r="AN73" s="95"/>
+      <c r="AO73" s="95"/>
+      <c r="AP73" s="95"/>
+      <c r="AQ73" s="95"/>
+      <c r="AR73" s="95"/>
+      <c r="AS73" s="95"/>
+      <c r="AT73" s="95"/>
+      <c r="AU73" s="95"/>
+      <c r="AV73" s="95"/>
+      <c r="AW73" s="95"/>
+      <c r="AX73" s="95"/>
+      <c r="AY73" s="95"/>
+      <c r="AZ73" s="95"/>
+      <c r="BA73" s="95"/>
+      <c r="BB73" s="95"/>
+      <c r="BC73" s="95"/>
+      <c r="BD73" s="95"/>
+      <c r="BE73" s="95"/>
+      <c r="BF73" s="95"/>
+      <c r="BG73" s="95"/>
+      <c r="BH73" s="95"/>
+      <c r="BI73" s="95"/>
+      <c r="BJ73" s="95"/>
+      <c r="BK73" s="95"/>
+      <c r="BL73" s="95"/>
+      <c r="BM73" s="95"/>
+      <c r="BN73" s="95"/>
+      <c r="BO73" s="95"/>
+      <c r="BP73" s="95"/>
+      <c r="BQ73" s="95"/>
+      <c r="BR73" s="95"/>
+      <c r="BS73" s="95"/>
+      <c r="BT73" s="95"/>
+      <c r="BU73" s="95"/>
+      <c r="BV73" s="95"/>
+      <c r="BW73" s="95"/>
+      <c r="BX73" s="95"/>
+      <c r="BY73" s="95"/>
+      <c r="BZ73" s="95"/>
+      <c r="CA73" s="95"/>
+      <c r="CB73" s="95"/>
+      <c r="CC73" s="95"/>
+      <c r="CD73" s="95"/>
+      <c r="CE73" s="95"/>
+      <c r="CF73" s="95"/>
+      <c r="CG73" s="95"/>
+      <c r="CH73" s="95"/>
+      <c r="CI73" s="95"/>
+      <c r="CJ73" s="95"/>
+      <c r="CK73" s="95"/>
+      <c r="CL73" s="95"/>
+      <c r="CM73" s="95"/>
+      <c r="CN73" s="95"/>
+      <c r="CO73" s="95"/>
+      <c r="CP73" s="95"/>
+      <c r="CQ73" s="95"/>
+      <c r="CR73" s="95"/>
+      <c r="CS73" s="95"/>
+      <c r="CT73" s="95"/>
+      <c r="CU73" s="95"/>
+      <c r="CV73" s="95"/>
+      <c r="CW73" s="95"/>
+      <c r="CX73" s="95"/>
+      <c r="CY73" s="95"/>
+      <c r="CZ73" s="95"/>
+      <c r="DA73" s="95"/>
+      <c r="DB73" s="95"/>
+      <c r="DC73" s="95"/>
+      <c r="DD73" s="95"/>
+      <c r="DE73" s="95"/>
+      <c r="DF73" s="95"/>
+      <c r="DG73" s="95"/>
+      <c r="DH73" s="95"/>
+      <c r="DI73" s="95"/>
+      <c r="DJ73" s="95"/>
+      <c r="DK73" s="95"/>
+      <c r="DL73" s="95"/>
+      <c r="DM73" s="95"/>
+      <c r="DN73" s="95"/>
+      <c r="DO73" s="95"/>
+      <c r="DP73" s="95"/>
+      <c r="DQ73" s="95"/>
+      <c r="DR73" s="95"/>
+      <c r="DS73" s="95"/>
+      <c r="DT73" s="95"/>
+      <c r="DU73" s="95"/>
+      <c r="DV73" s="95"/>
+      <c r="DW73" s="95"/>
+      <c r="DX73" s="95"/>
+      <c r="DY73" s="95"/>
+      <c r="DZ73" s="95"/>
+      <c r="EA73" s="95"/>
+      <c r="EB73" s="95"/>
+      <c r="EC73" s="95"/>
+      <c r="ED73" s="95"/>
+      <c r="EE73" s="95"/>
+      <c r="EF73" s="95"/>
+      <c r="EG73" s="95"/>
+      <c r="EH73" s="95"/>
+      <c r="EI73" s="95"/>
+      <c r="EJ73" s="95"/>
+      <c r="EK73" s="95"/>
+      <c r="EL73" s="95"/>
+      <c r="EM73" s="95"/>
+      <c r="EN73" s="95"/>
+      <c r="EO73" s="95"/>
+      <c r="EP73" s="95"/>
+      <c r="EQ73" s="95"/>
+      <c r="ER73" s="95"/>
+      <c r="ES73" s="95"/>
+      <c r="ET73" s="95"/>
+      <c r="EU73" s="95"/>
+      <c r="EV73" s="95"/>
+      <c r="EW73" s="95"/>
+      <c r="EX73" s="95"/>
+      <c r="EY73" s="95"/>
+      <c r="EZ73" s="95"/>
+      <c r="FA73" s="95"/>
+      <c r="FB73" s="95"/>
+      <c r="FC73" s="95"/>
+      <c r="FD73" s="95"/>
+      <c r="FE73" s="95"/>
+      <c r="FF73" s="95"/>
+      <c r="FG73" s="95"/>
+      <c r="FH73" s="95"/>
+      <c r="FI73" s="95"/>
+      <c r="FJ73" s="95"/>
+      <c r="FK73" s="95"/>
+      <c r="FL73" s="95"/>
+      <c r="FM73" s="95"/>
+      <c r="FN73" s="95"/>
+      <c r="FO73" s="95"/>
+      <c r="FP73" s="95"/>
+      <c r="FQ73" s="95"/>
+      <c r="FR73" s="95"/>
+      <c r="FS73" s="95"/>
+      <c r="FT73" s="95"/>
+      <c r="FU73" s="95"/>
+      <c r="FV73" s="95"/>
+      <c r="FW73" s="95"/>
+      <c r="FX73" s="95"/>
+      <c r="FY73" s="95"/>
+      <c r="FZ73" s="95"/>
+      <c r="GA73" s="95"/>
+      <c r="GB73" s="95"/>
+      <c r="GC73" s="95"/>
+      <c r="GD73" s="95"/>
+      <c r="GE73" s="95"/>
+      <c r="GF73" s="95"/>
+      <c r="GG73" s="95"/>
+      <c r="GH73" s="95"/>
+      <c r="GI73" s="95"/>
+      <c r="GJ73" s="95"/>
+      <c r="GK73" s="95"/>
+      <c r="GL73" s="95"/>
+      <c r="GM73" s="95"/>
+      <c r="GN73" s="95"/>
+      <c r="GO73" s="95"/>
+      <c r="GP73" s="95"/>
+      <c r="GQ73" s="95"/>
+      <c r="GR73" s="95"/>
+      <c r="GS73" s="95"/>
+      <c r="GT73" s="95"/>
+      <c r="GU73" s="95"/>
+      <c r="GV73" s="95"/>
+      <c r="GW73" s="95"/>
+      <c r="GX73" s="95"/>
+      <c r="GY73" s="95"/>
+      <c r="GZ73" s="95"/>
+      <c r="HA73" s="95"/>
+      <c r="HB73" s="95"/>
+      <c r="HC73" s="95"/>
+      <c r="HD73" s="95"/>
+      <c r="HE73" s="95"/>
+      <c r="HF73" s="95"/>
+      <c r="HG73" s="95"/>
+      <c r="HH73" s="95"/>
+      <c r="HI73" s="95"/>
+      <c r="HJ73" s="95"/>
+      <c r="HK73" s="95"/>
+      <c r="HL73" s="95"/>
+      <c r="HM73" s="95"/>
+      <c r="HN73" s="95"/>
+      <c r="HO73" s="95"/>
+      <c r="HP73" s="95"/>
+      <c r="HQ73" s="95"/>
+      <c r="HR73" s="95"/>
+      <c r="HS73" s="95"/>
+      <c r="HT73" s="95"/>
+      <c r="HU73" s="95"/>
+      <c r="HV73" s="95"/>
+      <c r="HW73" s="95"/>
+      <c r="HX73" s="95"/>
+      <c r="HY73" s="95"/>
+      <c r="HZ73" s="95"/>
+      <c r="IA73" s="95"/>
+      <c r="IB73" s="95"/>
+      <c r="IC73" s="95"/>
+      <c r="ID73" s="95"/>
+      <c r="IE73" s="95"/>
+      <c r="IF73" s="95"/>
+      <c r="IG73" s="95"/>
+      <c r="IH73" s="95"/>
+      <c r="II73" s="95"/>
+      <c r="IJ73" s="95"/>
+      <c r="IK73" s="95"/>
+      <c r="IL73" s="95"/>
+      <c r="IM73" s="95"/>
+      <c r="IN73" s="95"/>
+      <c r="IO73" s="95"/>
+      <c r="IP73" s="95"/>
+      <c r="IQ73" s="95"/>
+      <c r="IR73" s="95"/>
+      <c r="IS73" s="95"/>
+      <c r="IT73" s="95"/>
+      <c r="IU73" s="95"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C73">
@@ -5990,27 +5987,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="111" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="75" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="75" t="s">
+      <c r="D1" s="112"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="76"/>
-      <c r="H1" s="75" t="s">
+      <c r="G1" s="108"/>
+      <c r="H1" s="107" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="76"/>
-      <c r="J1" s="75" t="s">
+      <c r="I1" s="108"/>
+      <c r="J1" s="107" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="76"/>
+      <c r="K1" s="108"/>
       <c r="L1" s="40"/>
       <c r="M1" s="13"/>
       <c r="N1" s="47"/>
@@ -6300,7 +6297,7 @@
       </c>
       <c r="J8" s="18">
         <f>COUNTIF(Junk!A1:A75,A8)+COUNTIF(Junk!Q1:T75,A8)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="54" t="e">
         <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A8)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A8)</f>
@@ -6308,7 +6305,7 @@
       </c>
       <c r="L8" s="18">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M8" s="15" t="e">
         <f t="shared" si="1"/>
@@ -6514,14 +6511,14 @@
       <c r="E13" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="G13" s="76"/>
-      <c r="H13" s="77" t="s">
+      <c r="G13" s="108"/>
+      <c r="H13" s="109" t="s">
         <v>138</v>
       </c>
-      <c r="I13" s="78"/>
+      <c r="I13" s="110"/>
       <c r="J13" s="53"/>
       <c r="K13" s="11"/>
       <c r="L13" s="8"/>

</xml_diff>

<commit_message>
Working on convert bonuses
</commit_message>
<xml_diff>
--- a/deck.xlsx
+++ b/deck.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="149">
   <si>
     <t>Type</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Friend 2</t>
   </si>
   <si>
-    <t>Bonus Conjunction</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>take wood</t>
   </si>
   <si>
-    <t xml:space="preserve">OR </t>
-  </si>
-  <si>
     <t>take metal</t>
   </si>
   <si>
@@ -216,9 +210,6 @@
     <t>convert anything to glass</t>
   </si>
   <si>
-    <t>TO</t>
-  </si>
-  <si>
     <t>Junk Store</t>
   </si>
   <si>
@@ -454,6 +445,24 @@
   </si>
   <si>
     <t>take wood or metal</t>
+  </si>
+  <si>
+    <t>Convert</t>
+  </si>
+  <si>
+    <t>convert</t>
+  </si>
+  <si>
+    <t>ConvNum</t>
+  </si>
+  <si>
+    <t>ConvType</t>
+  </si>
+  <si>
+    <t>Conv2Num</t>
+  </si>
+  <si>
+    <t>Conv2Type</t>
   </si>
 </sst>
 </file>
@@ -940,7 +949,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1213,6 +1222,12 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2583,10 +2598,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IU73"/>
+  <dimension ref="A1:IT73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -2605,13 +2622,15 @@
     <col min="12" max="12" width="7" style="1" customWidth="1"/>
     <col min="13" max="13" width="8.5" style="93" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="255" width="6.59765625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.59765625" style="114" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6.796875" style="114" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="7.5" style="114" bestFit="1" customWidth="1"/>
+    <col min="22" max="254" width="6.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="81" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:254" s="81" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2634,7 +2653,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="104" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I1" s="88" t="s">
         <v>8</v>
@@ -2649,24 +2668,32 @@
         <v>11</v>
       </c>
       <c r="M1" s="88" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="79" t="s">
-        <v>142</v>
-      </c>
-      <c r="O1" s="79" t="s">
-        <v>12</v>
-      </c>
       <c r="P1" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" s="79" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
+      <c r="R1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="V1" s="80"/>
       <c r="W1" s="80"/>
       <c r="X1" s="80"/>
@@ -2900,17 +2927,16 @@
       <c r="IR1" s="80"/>
       <c r="IS1" s="80"/>
       <c r="IT1" s="80"/>
-      <c r="IU1" s="80"/>
-    </row>
-    <row r="2" spans="1:255" ht="17.100000000000001" customHeight="1">
+    </row>
+    <row r="2" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="C2" s="98" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="98" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="101"/>
       <c r="E2" s="77"/>
@@ -2927,21 +2953,25 @@
         <v>1</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O2" s="77"/>
       <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-    </row>
-    <row r="3" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q2" s="113"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="113"/>
+    </row>
+    <row r="3" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="91"/>
       <c r="E3" s="15">
@@ -2960,21 +2990,25 @@
         <v>1</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q3" s="21"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="21"/>
+    </row>
+    <row r="4" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="91"/>
       <c r="E4" s="15">
@@ -2995,21 +3029,25 @@
         <v>2</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q4" s="21"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="21"/>
+    </row>
+    <row r="5" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="90">
         <v>3</v>
@@ -3028,21 +3066,25 @@
         <v>2</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q5" s="21"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="21"/>
+    </row>
+    <row r="6" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="91"/>
       <c r="E6" s="8"/>
@@ -3059,25 +3101,29 @@
         <v>1</v>
       </c>
       <c r="N6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="15">
+        <v>1</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+    </row>
+    <row r="7" spans="1:254" ht="17.100000000000001" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:255" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="91"/>
       <c r="E7" s="15">
@@ -3096,25 +3142,29 @@
         <v>1</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:255" ht="17.100000000000001" customHeight="1">
+        <v>21</v>
+      </c>
+      <c r="O7" s="15">
+        <v>1</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+    </row>
+    <row r="8" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="90">
         <v>2</v>
@@ -3135,21 +3185,25 @@
         <v>2</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-    </row>
-    <row r="9" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q8" s="21"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="21"/>
+    </row>
+    <row r="9" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="90">
         <v>2</v>
@@ -3168,21 +3222,25 @@
         <v>1</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-    </row>
-    <row r="10" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q9" s="21"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="21"/>
+    </row>
+    <row r="10" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="90">
         <v>5</v>
@@ -3199,21 +3257,25 @@
         <v>1</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-    </row>
-    <row r="11" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q10" s="21"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="21"/>
+    </row>
+    <row r="11" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="90">
         <v>3</v>
@@ -3232,21 +3294,25 @@
         <v>1</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-    </row>
-    <row r="12" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q11" s="21"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="21"/>
+    </row>
+    <row r="12" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="90">
         <v>2</v>
@@ -3265,25 +3331,29 @@
         <v>1</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" s="8"/>
-      <c r="P12" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:255" ht="17.100000000000001" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="O12" s="15">
+        <v>1</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+    </row>
+    <row r="13" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="91"/>
       <c r="E13" s="15">
@@ -3302,17 +3372,21 @@
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-    </row>
-    <row r="14" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q13" s="21"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="21"/>
+    </row>
+    <row r="14" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="90">
         <v>2</v>
@@ -3331,25 +3405,29 @@
         <v>1</v>
       </c>
       <c r="N14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="15">
+        <v>1</v>
+      </c>
+      <c r="P14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="8"/>
-      <c r="P14" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+    </row>
+    <row r="15" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="91"/>
       <c r="E15" s="15">
@@ -3370,21 +3448,25 @@
         <v>1</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-    </row>
-    <row r="16" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q15" s="21"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="21"/>
+    </row>
+    <row r="16" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="91"/>
       <c r="E16" s="15">
@@ -3405,21 +3487,25 @@
         <v>1</v>
       </c>
       <c r="N16" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-    </row>
-    <row r="17" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q16" s="21"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="21"/>
+    </row>
+    <row r="17" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="91"/>
       <c r="E17" s="8"/>
@@ -3436,21 +3522,25 @@
         <v>1</v>
       </c>
       <c r="N17" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-    </row>
-    <row r="18" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q17" s="21"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="21"/>
+    </row>
+    <row r="18" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="90">
         <v>3</v>
@@ -3469,17 +3559,21 @@
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-    </row>
-    <row r="19" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q18" s="21"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="21"/>
+    </row>
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="91"/>
       <c r="E19" s="8"/>
@@ -3498,21 +3592,25 @@
         <v>1</v>
       </c>
       <c r="N19" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-    </row>
-    <row r="20" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q19" s="21"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="21"/>
+    </row>
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="91"/>
       <c r="E20" s="15">
@@ -3531,21 +3629,25 @@
         <v>1</v>
       </c>
       <c r="N20" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="14"/>
-    </row>
-    <row r="21" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="P20" s="14"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+    </row>
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="90">
         <v>4</v>
@@ -3564,17 +3666,21 @@
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-    </row>
-    <row r="22" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q21" s="21"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="21"/>
+    </row>
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="90">
         <v>2</v>
@@ -3595,21 +3701,25 @@
         <v>1</v>
       </c>
       <c r="N22" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-    </row>
-    <row r="23" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q22" s="21"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="21"/>
+    </row>
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="90">
         <v>3</v>
@@ -3630,17 +3740,21 @@
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-    </row>
-    <row r="24" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q23" s="21"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="21"/>
+    </row>
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="90">
         <v>3</v>
@@ -3661,21 +3775,25 @@
         <v>1</v>
       </c>
       <c r="N24" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-    </row>
-    <row r="25" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q24" s="21"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="21"/>
+    </row>
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="90">
         <v>2</v>
@@ -3696,17 +3814,21 @@
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-    </row>
-    <row r="26" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q25" s="21"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="21"/>
+    </row>
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="90">
         <v>2</v>
@@ -3725,21 +3847,25 @@
         <v>2</v>
       </c>
       <c r="N26" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-    </row>
-    <row r="27" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q26" s="21"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="21"/>
+    </row>
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D27" s="91"/>
       <c r="E27" s="8"/>
@@ -3758,17 +3884,21 @@
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-    </row>
-    <row r="28" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q27" s="21"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="21"/>
+    </row>
+    <row r="28" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D28" s="90">
         <v>5</v>
@@ -3785,21 +3915,25 @@
         <v>2</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-    </row>
-    <row r="29" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q28" s="21"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="21"/>
+    </row>
+    <row r="29" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D29" s="90">
         <v>2</v>
@@ -3818,21 +3952,25 @@
         <v>1</v>
       </c>
       <c r="N29" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-    </row>
-    <row r="30" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q29" s="21"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="21"/>
+    </row>
+    <row r="30" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D30" s="91"/>
       <c r="E30" s="15">
@@ -3851,21 +3989,25 @@
         <v>1</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-    </row>
-    <row r="31" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q30" s="21"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="21"/>
+    </row>
+    <row r="31" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D31" s="90">
         <v>1</v>
@@ -3886,21 +4028,25 @@
         <v>2</v>
       </c>
       <c r="N31" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-    </row>
-    <row r="32" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q31" s="21"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="21"/>
+    </row>
+    <row r="32" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D32" s="90">
         <v>3</v>
@@ -3919,21 +4065,25 @@
         <v>1</v>
       </c>
       <c r="N32" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-    </row>
-    <row r="33" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q32" s="21"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="21"/>
+    </row>
+    <row r="33" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33" s="91"/>
       <c r="E33" s="15">
@@ -3952,21 +4102,25 @@
         <v>1</v>
       </c>
       <c r="N33" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-    </row>
-    <row r="34" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q33" s="21"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="21"/>
+    </row>
+    <row r="34" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D34" s="90">
         <v>3</v>
@@ -3987,17 +4141,21 @@
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-    </row>
-    <row r="35" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q34" s="21"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="21"/>
+    </row>
+    <row r="35" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D35" s="90">
         <v>2</v>
@@ -4018,17 +4176,21 @@
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-    </row>
-    <row r="36" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q35" s="21"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="21"/>
+    </row>
+    <row r="36" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C36" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="91"/>
       <c r="E36" s="8"/>
@@ -4047,25 +4209,29 @@
         <v>1</v>
       </c>
       <c r="N36" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O36" s="15">
+        <v>1</v>
+      </c>
+      <c r="P36" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O36" s="8"/>
-      <c r="P36" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+    </row>
+    <row r="37" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>60</v>
-      </c>
       <c r="C37" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37" s="91"/>
       <c r="E37" s="15">
@@ -4084,25 +4250,29 @@
         <v>1</v>
       </c>
       <c r="N37" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O37" s="15">
+        <v>1</v>
+      </c>
+      <c r="P37" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="8"/>
-      <c r="P37" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+    </row>
+    <row r="38" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" s="91"/>
       <c r="E38" s="15">
@@ -4123,25 +4293,29 @@
         <v>2</v>
       </c>
       <c r="N38" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O38" s="8"/>
-      <c r="P38" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q38" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="17.100000000000001" customHeight="1">
+        <v>21</v>
+      </c>
+      <c r="O38" s="15">
+        <v>2</v>
+      </c>
+      <c r="P38" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+    </row>
+    <row r="39" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C39" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D39" s="90">
         <v>2</v>
@@ -4162,25 +4336,29 @@
         <v>3</v>
       </c>
       <c r="N39" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="O39" s="8"/>
-      <c r="P39" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="17.100000000000001" customHeight="1">
+        <v>38</v>
+      </c>
+      <c r="O39" s="15">
+        <v>1</v>
+      </c>
+      <c r="P39" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="15"/>
+    </row>
+    <row r="40" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C40" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D40" s="91"/>
       <c r="E40" s="8"/>
@@ -4197,25 +4375,29 @@
         <v>2</v>
       </c>
       <c r="N40" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O40" s="8"/>
-      <c r="P40" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q40" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="17.100000000000001" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="O40" s="15">
+        <v>2</v>
+      </c>
+      <c r="P40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+    </row>
+    <row r="41" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D41" s="90">
         <v>2</v>
@@ -4232,27 +4414,35 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="84"/>
-      <c r="M41" s="90">
-        <v>1</v>
-      </c>
-      <c r="N41" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="O41" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="8"/>
-    </row>
-    <row r="42" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="M41" s="90"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="R41" s="15">
+        <v>1</v>
+      </c>
+      <c r="S41" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T41" s="15">
+        <v>1</v>
+      </c>
+      <c r="U41" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C42" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D42" s="90">
         <v>2</v>
@@ -4269,27 +4459,35 @@
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="84"/>
-      <c r="M42" s="90">
-        <v>1</v>
-      </c>
-      <c r="N42" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="O42" s="15" t="s">
+      <c r="M42" s="90"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="R42" s="15">
+        <v>1</v>
+      </c>
+      <c r="S42" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T42" s="15">
+        <v>1</v>
+      </c>
+      <c r="U42" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="17.100000000000001" customHeight="1">
+      <c r="A43" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="8"/>
-    </row>
-    <row r="43" spans="1:17" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>69</v>
-      </c>
       <c r="C43" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="91"/>
       <c r="E43" s="8"/>
@@ -4310,21 +4508,25 @@
         <v>3</v>
       </c>
       <c r="N43" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O43" s="8"/>
       <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-    </row>
-    <row r="44" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q43" s="21"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="21"/>
+    </row>
+    <row r="44" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C44" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D44" s="91"/>
       <c r="E44" s="15">
@@ -4345,21 +4547,25 @@
         <v>3</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O44" s="8"/>
       <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-    </row>
-    <row r="45" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q44" s="21"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="21"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="21"/>
+    </row>
+    <row r="45" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C45" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D45" s="90">
         <v>4</v>
@@ -4378,21 +4584,25 @@
         <v>3</v>
       </c>
       <c r="N45" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O45" s="8"/>
       <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-    </row>
-    <row r="46" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q45" s="21"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="21"/>
+    </row>
+    <row r="46" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C46" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D46" s="90">
         <v>4</v>
@@ -4409,21 +4619,25 @@
         <v>2</v>
       </c>
       <c r="N46" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O46" s="8"/>
       <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-    </row>
-    <row r="47" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q46" s="21"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="21"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="21"/>
+    </row>
+    <row r="47" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C47" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D47" s="90">
         <v>2</v>
@@ -4442,25 +4656,29 @@
         <v>2</v>
       </c>
       <c r="N47" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O47" s="8"/>
-      <c r="P47" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="17.100000000000001" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="O47" s="15">
+        <v>1</v>
+      </c>
+      <c r="P47" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+    </row>
+    <row r="48" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C48" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D48" s="90">
         <v>12</v>
@@ -4479,21 +4697,25 @@
       <c r="L48" s="84"/>
       <c r="M48" s="91"/>
       <c r="N48" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O48" s="8"/>
       <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-    </row>
-    <row r="49" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q48" s="21"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="21"/>
+    </row>
+    <row r="49" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C49" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" s="91"/>
       <c r="E49" s="15">
@@ -4512,21 +4734,25 @@
       <c r="L49" s="84"/>
       <c r="M49" s="91"/>
       <c r="N49" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O49" s="8"/>
       <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-    </row>
-    <row r="50" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q49" s="21"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="21"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="21"/>
+    </row>
+    <row r="50" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="C50" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D50" s="90">
         <v>12</v>
@@ -4545,21 +4771,25 @@
       <c r="L50" s="84"/>
       <c r="M50" s="91"/>
       <c r="N50" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O50" s="8"/>
       <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-    </row>
-    <row r="51" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q50" s="21"/>
+      <c r="R50" s="15"/>
+      <c r="S50" s="21"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="21"/>
+    </row>
+    <row r="51" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C51" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D51" s="91"/>
       <c r="E51" s="8"/>
@@ -4578,21 +4808,25 @@
       <c r="L51" s="84"/>
       <c r="M51" s="91"/>
       <c r="N51" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O51" s="8"/>
       <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
-    </row>
-    <row r="52" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q51" s="21"/>
+      <c r="R51" s="15"/>
+      <c r="S51" s="21"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="21"/>
+    </row>
+    <row r="52" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C52" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D52" s="91"/>
       <c r="E52" s="15">
@@ -4611,21 +4845,25 @@
       <c r="L52" s="84"/>
       <c r="M52" s="91"/>
       <c r="N52" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O52" s="8"/>
       <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
-    </row>
-    <row r="53" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q52" s="21"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="21"/>
+      <c r="T52" s="15"/>
+      <c r="U52" s="21"/>
+    </row>
+    <row r="53" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C53" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D53" s="90">
         <v>2</v>
@@ -4644,25 +4882,29 @@
         <v>2</v>
       </c>
       <c r="N53" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O53" s="15">
+        <v>1</v>
+      </c>
+      <c r="P53" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O53" s="8"/>
-      <c r="P53" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q53" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="15"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="15"/>
+    </row>
+    <row r="54" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C54" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D54" s="91"/>
       <c r="E54" s="8"/>
@@ -4679,25 +4921,29 @@
         <v>1</v>
       </c>
       <c r="N54" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="O54" s="8"/>
-      <c r="P54" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q54" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" ht="17.100000000000001" customHeight="1">
+        <v>15</v>
+      </c>
+      <c r="O54" s="15">
+        <v>1</v>
+      </c>
+      <c r="P54" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+    </row>
+    <row r="55" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C55" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D55" s="91"/>
       <c r="E55" s="15">
@@ -4714,25 +4960,29 @@
         <v>1</v>
       </c>
       <c r="N55" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="O55" s="8"/>
-      <c r="P55" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q55" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" ht="17.100000000000001" customHeight="1">
+        <v>15</v>
+      </c>
+      <c r="O55" s="15">
+        <v>1</v>
+      </c>
+      <c r="P55" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="15"/>
+      <c r="T55" s="15"/>
+      <c r="U55" s="15"/>
+    </row>
+    <row r="56" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C56" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D56" s="90">
         <v>2</v>
@@ -4751,29 +5001,35 @@
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
       <c r="L56" s="84"/>
-      <c r="M56" s="90">
-        <v>1</v>
-      </c>
-      <c r="N56" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="O56" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P56" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q56" s="8"/>
-    </row>
-    <row r="57" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="M56" s="90"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="15"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R56" s="15">
+        <v>1</v>
+      </c>
+      <c r="S56" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T56" s="15">
+        <v>1</v>
+      </c>
+      <c r="U56" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C57" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D57" s="91"/>
       <c r="E57" s="8"/>
@@ -4790,21 +5046,25 @@
         <v>2</v>
       </c>
       <c r="N57" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O57" s="8"/>
       <c r="P57" s="8"/>
-      <c r="Q57" s="8"/>
-    </row>
-    <row r="58" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q57" s="21"/>
+      <c r="R57" s="15"/>
+      <c r="S57" s="21"/>
+      <c r="T57" s="15"/>
+      <c r="U57" s="21"/>
+    </row>
+    <row r="58" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A58" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C58" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D58" s="91"/>
       <c r="E58" s="15">
@@ -4823,25 +5083,29 @@
         <v>1</v>
       </c>
       <c r="N58" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O58" s="8"/>
-      <c r="P58" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q58" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="17.100000000000001" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="O58" s="15">
+        <v>1</v>
+      </c>
+      <c r="P58" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q58" s="15"/>
+      <c r="R58" s="15"/>
+      <c r="S58" s="15"/>
+      <c r="T58" s="15"/>
+      <c r="U58" s="15"/>
+    </row>
+    <row r="59" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A59" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C59" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59" s="91"/>
       <c r="E59" s="8"/>
@@ -4852,29 +5116,35 @@
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
       <c r="L59" s="84"/>
-      <c r="M59" s="90">
-        <v>2</v>
-      </c>
-      <c r="N59" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="O59" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P59" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q59" s="8"/>
-    </row>
-    <row r="60" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="M59" s="90"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R59" s="15">
+        <v>2</v>
+      </c>
+      <c r="S59" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T59" s="15">
+        <v>1</v>
+      </c>
+      <c r="U59" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A60" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C60" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D60" s="91"/>
       <c r="E60" s="8"/>
@@ -4893,29 +5163,35 @@
       <c r="L60" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="M60" s="90">
-        <v>1</v>
-      </c>
-      <c r="N60" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="O60" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P60" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q60" s="8"/>
-    </row>
-    <row r="61" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="M60" s="90"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R60" s="15">
+        <v>1</v>
+      </c>
+      <c r="S60" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T60" s="15">
+        <v>1</v>
+      </c>
+      <c r="U60" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A61" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B61" s="17" t="s">
-        <v>90</v>
-      </c>
       <c r="C61" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61" s="91"/>
       <c r="E61" s="8"/>
@@ -4930,29 +5206,35 @@
       </c>
       <c r="K61" s="21"/>
       <c r="L61" s="84"/>
-      <c r="M61" s="90">
-        <v>1</v>
-      </c>
-      <c r="N61" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="O61" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P61" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q61" s="8"/>
-    </row>
-    <row r="62" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="M61" s="90"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R61" s="15">
+        <v>1</v>
+      </c>
+      <c r="S61" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T61" s="15">
+        <v>2</v>
+      </c>
+      <c r="U61" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A62" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C62" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D62" s="91"/>
       <c r="E62" s="8"/>
@@ -4967,21 +5249,25 @@
         <v>1</v>
       </c>
       <c r="N62" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O62" s="8"/>
       <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
-    </row>
-    <row r="63" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="Q62" s="21"/>
+      <c r="R62" s="15"/>
+      <c r="S62" s="21"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="21"/>
+    </row>
+    <row r="63" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A63" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C63" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D63" s="91"/>
       <c r="E63" s="8"/>
@@ -4996,29 +5282,35 @@
       </c>
       <c r="K63" s="21"/>
       <c r="L63" s="84"/>
-      <c r="M63" s="90">
-        <v>1</v>
-      </c>
-      <c r="N63" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="O63" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P63" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q63" s="8"/>
-    </row>
-    <row r="64" spans="1:17" ht="17.100000000000001" customHeight="1">
+      <c r="M63" s="90"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R63" s="15">
+        <v>1</v>
+      </c>
+      <c r="S63" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="T63" s="15">
+        <v>1</v>
+      </c>
+      <c r="U63" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A64" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C64" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D64" s="91"/>
       <c r="E64" s="8"/>
@@ -5033,21 +5325,25 @@
         <v>1</v>
       </c>
       <c r="N64" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O64" s="8"/>
       <c r="P64" s="8"/>
-      <c r="Q64" s="8"/>
-    </row>
-    <row r="65" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="Q64" s="21"/>
+      <c r="R64" s="15"/>
+      <c r="S64" s="21"/>
+      <c r="T64" s="15"/>
+      <c r="U64" s="21"/>
+    </row>
+    <row r="65" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A65" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C65" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D65" s="91"/>
       <c r="E65" s="8"/>
@@ -5062,29 +5358,35 @@
       </c>
       <c r="K65" s="21"/>
       <c r="L65" s="84"/>
-      <c r="M65" s="90">
-        <v>1</v>
-      </c>
-      <c r="N65" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="O65" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P65" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="8"/>
-    </row>
-    <row r="66" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="M65" s="90"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R65" s="15">
+        <v>1</v>
+      </c>
+      <c r="S65" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="T65" s="15">
+        <v>1</v>
+      </c>
+      <c r="U65" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A66" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C66" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D66" s="91"/>
       <c r="E66" s="8"/>
@@ -5103,27 +5405,29 @@
         <v>1</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O66" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="P66" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q66" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="1:255" ht="17.100000000000001" customHeight="1">
+        <v>38</v>
+      </c>
+      <c r="O66" s="15">
+        <v>1</v>
+      </c>
+      <c r="P66" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="15"/>
+      <c r="S66" s="15"/>
+      <c r="T66" s="15"/>
+      <c r="U66" s="15"/>
+    </row>
+    <row r="67" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A67" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C67" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67" s="91"/>
       <c r="E67" s="8"/>
@@ -5142,25 +5446,29 @@
         <v>1</v>
       </c>
       <c r="N67" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O67" s="8"/>
-      <c r="P67" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q67" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="68" spans="1:255" ht="17.100000000000001" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="O67" s="15">
+        <v>1</v>
+      </c>
+      <c r="P67" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
+      <c r="S67" s="15"/>
+      <c r="T67" s="15"/>
+      <c r="U67" s="15"/>
+    </row>
+    <row r="68" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A68" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C68" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D68" s="91"/>
       <c r="E68" s="8"/>
@@ -5175,29 +5483,35 @@
       </c>
       <c r="K68" s="21"/>
       <c r="L68" s="84"/>
-      <c r="M68" s="90">
-        <v>1</v>
-      </c>
-      <c r="N68" s="14" t="s">
+      <c r="M68" s="90"/>
+      <c r="N68" s="14"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R68" s="15">
+        <v>1</v>
+      </c>
+      <c r="S68" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T68" s="15">
+        <v>1</v>
+      </c>
+      <c r="U68" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:254" ht="17.100000000000001" customHeight="1">
+      <c r="A69" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="O68" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P68" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="8"/>
-    </row>
-    <row r="69" spans="1:255" ht="17.100000000000001" customHeight="1">
-      <c r="A69" s="16" t="s">
-        <v>87</v>
-      </c>
       <c r="B69" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C69" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D69" s="91"/>
       <c r="E69" s="8"/>
@@ -5216,29 +5530,35 @@
       <c r="L69" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="M69" s="90">
-        <v>1</v>
-      </c>
-      <c r="N69" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="O69" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P69" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q69" s="8"/>
-    </row>
-    <row r="70" spans="1:255" ht="17.100000000000001" customHeight="1">
+      <c r="M69" s="90"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="8"/>
+      <c r="Q69" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R69" s="15">
+        <v>1</v>
+      </c>
+      <c r="S69" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T69" s="15">
+        <v>1</v>
+      </c>
+      <c r="U69" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A70" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C70" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D70" s="102"/>
       <c r="E70" s="21"/>
@@ -5253,21 +5573,25 @@
         <v>1</v>
       </c>
       <c r="N70" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="O70" s="24"/>
-      <c r="P70" s="21"/>
-      <c r="Q70" s="25"/>
-    </row>
-    <row r="71" spans="1:255" ht="17.100000000000001" customHeight="1">
+        <v>100</v>
+      </c>
+      <c r="O70" s="21"/>
+      <c r="P70" s="25"/>
+      <c r="Q70" s="21"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="21"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="21"/>
+    </row>
+    <row r="71" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A71" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C71" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D71" s="102"/>
       <c r="E71" s="8"/>
@@ -5282,31 +5606,35 @@
       </c>
       <c r="K71" s="24"/>
       <c r="L71" s="86"/>
-      <c r="M71" s="90">
-        <v>1</v>
-      </c>
-      <c r="N71" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="O71" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P71" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q71" s="14" t="s">
+      <c r="M71" s="90"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="14"/>
+      <c r="Q71" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R71" s="15">
+        <v>1</v>
+      </c>
+      <c r="S71" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="T71" s="15">
+        <v>1</v>
+      </c>
+      <c r="U71" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:255" ht="17.100000000000001" customHeight="1">
+    <row r="72" spans="1:254" ht="17.100000000000001" customHeight="1">
       <c r="A72" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C72" s="99" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D72" s="102"/>
       <c r="E72" s="8"/>
@@ -5321,29 +5649,35 @@
       </c>
       <c r="K72" s="24"/>
       <c r="L72" s="86"/>
-      <c r="M72" s="90">
-        <v>1</v>
-      </c>
-      <c r="N72" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="O72" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="P72" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q72" s="25"/>
-    </row>
-    <row r="73" spans="1:255" s="96" customFormat="1" ht="15.75" customHeight="1">
+      <c r="M72" s="90"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="25"/>
+      <c r="Q72" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="R72" s="15">
+        <v>1</v>
+      </c>
+      <c r="S72" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="T72" s="15">
+        <v>1</v>
+      </c>
+      <c r="U72" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:254" s="96" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C73" s="100" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D73" s="103"/>
       <c r="E73" s="29"/>
@@ -5362,19 +5696,19 @@
         <v>1</v>
       </c>
       <c r="N73" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="O73" s="29"/>
-      <c r="P73" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="R73" s="95"/>
-      <c r="S73" s="95"/>
-      <c r="T73" s="95"/>
-      <c r="U73" s="95"/>
+        <v>21</v>
+      </c>
+      <c r="O73" s="33">
+        <v>1</v>
+      </c>
+      <c r="P73" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q73" s="33"/>
+      <c r="R73" s="33"/>
+      <c r="S73" s="33"/>
+      <c r="T73" s="33"/>
+      <c r="U73" s="33"/>
       <c r="V73" s="95"/>
       <c r="W73" s="95"/>
       <c r="X73" s="95"/>
@@ -5608,7 +5942,6 @@
       <c r="IR73" s="95"/>
       <c r="IS73" s="95"/>
       <c r="IT73" s="95"/>
-      <c r="IU73" s="95"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C73">
@@ -5660,84 +5993,84 @@
         <v>0</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D3" s="40"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>111</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>114</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D5" s="40"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C7" s="40"/>
       <c r="D7" s="8"/>
@@ -5745,10 +6078,10 @@
     </row>
     <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C8" s="40"/>
       <c r="D8" s="8"/>
@@ -5756,10 +6089,10 @@
     </row>
     <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C9" s="40"/>
       <c r="D9" s="8"/>
@@ -5767,10 +6100,10 @@
     </row>
     <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C10" s="40"/>
       <c r="D10" s="8"/>
@@ -5778,10 +6111,10 @@
     </row>
     <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C11" s="40"/>
       <c r="D11" s="8"/>
@@ -5789,10 +6122,10 @@
     </row>
     <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C12" s="40"/>
       <c r="D12" s="8"/>
@@ -5800,10 +6133,10 @@
     </row>
     <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C13" s="40"/>
       <c r="D13" s="8"/>
@@ -5811,10 +6144,10 @@
     </row>
     <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C14" s="40"/>
       <c r="D14" s="8"/>
@@ -5822,10 +6155,10 @@
     </row>
     <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="8"/>
@@ -5833,10 +6166,10 @@
     </row>
     <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="8"/>
@@ -5844,10 +6177,10 @@
     </row>
     <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="8"/>
@@ -5855,10 +6188,10 @@
     </row>
     <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="8"/>
@@ -5866,10 +6199,10 @@
     </row>
     <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="8"/>
@@ -5877,13 +6210,13 @@
     </row>
     <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="8"/>
@@ -5893,10 +6226,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="8"/>
@@ -5906,10 +6239,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D22" s="40"/>
       <c r="E22" s="8"/>
@@ -5919,10 +6252,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>120</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>123</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="8"/>
@@ -5932,10 +6265,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="8"/>
@@ -5945,10 +6278,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D25" s="40"/>
       <c r="E25" s="8"/>
@@ -5988,24 +6321,24 @@
   <sheetData>
     <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="111" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="107" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D1" s="112"/>
       <c r="E1" s="108"/>
       <c r="F1" s="107" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G1" s="108"/>
       <c r="H1" s="107" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I1" s="108"/>
       <c r="J1" s="107" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K1" s="108"/>
       <c r="L1" s="40"/>
@@ -6024,37 +6357,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="N2" s="48"/>
       <c r="O2" s="8"/>
@@ -6079,11 +6412,11 @@
       <c r="H3" s="45"/>
       <c r="I3" s="52"/>
       <c r="J3" s="10">
-        <f>COUNTIF(Junk!A1:A75,A3)+COUNTIF(Junk!Q1:T75,A3)</f>
+        <f>COUNTIF(Junk!A1:A75,A3)+COUNTIF(Junk!P1:S75,A3)</f>
         <v>5</v>
       </c>
       <c r="K3" s="50" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A3)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A3)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A3)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A3)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L3" s="10">
@@ -6117,11 +6450,11 @@
       <c r="H4" s="22"/>
       <c r="I4" s="23"/>
       <c r="J4" s="18">
-        <f>COUNTIF(Junk!A1:A75,A4)+COUNTIF(Junk!Q1:T75,A4)</f>
+        <f>COUNTIF(Junk!A1:A75,A4)+COUNTIF(Junk!P1:S75,A4)</f>
         <v>1</v>
       </c>
       <c r="K4" s="54" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A4)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A4)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A4)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A4)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L4" s="18">
@@ -6149,11 +6482,11 @@
       <c r="H5" s="22"/>
       <c r="I5" s="23"/>
       <c r="J5" s="18">
-        <f>COUNTIF(Junk!A1:A75,A5)+COUNTIF(Junk!Q1:T75,A5)</f>
+        <f>COUNTIF(Junk!A1:A75,A5)+COUNTIF(Junk!P1:S75,A5)</f>
         <v>0</v>
       </c>
       <c r="K5" s="54" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A5)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A5)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A5)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A5)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L5" s="18">
@@ -6187,11 +6520,11 @@
       <c r="H6" s="28"/>
       <c r="I6" s="58"/>
       <c r="J6" s="31">
-        <f>COUNTIF(Junk!A1:A75,A6)+COUNTIF(Junk!Q1:T75,A6)</f>
+        <f>COUNTIF(Junk!A1:A75,A6)+COUNTIF(Junk!P1:S75,A6)</f>
         <v>2</v>
       </c>
       <c r="K6" s="56" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A6)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A6)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A6)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A6)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L6" s="31">
@@ -6241,11 +6574,11 @@
         <v>5</v>
       </c>
       <c r="J7" s="10">
-        <f>COUNTIF(Junk!A1:A75,A7)+COUNTIF(Junk!Q1:T75,A7)</f>
+        <f>COUNTIF(Junk!A1:A75,A7)+COUNTIF(Junk!P1:S75,A7)</f>
         <v>0</v>
       </c>
       <c r="K7" s="50" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A7)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A7)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A7)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A7)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L7" s="10">
@@ -6296,16 +6629,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="J8" s="18">
-        <f>COUNTIF(Junk!A1:A75,A8)+COUNTIF(Junk!Q1:T75,A8)</f>
-        <v>0</v>
+        <f>COUNTIF(Junk!A1:A75,A8)+COUNTIF(Junk!P1:S75,A8)</f>
+        <v>1</v>
       </c>
       <c r="K8" s="54" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A8)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A8)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A8)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A8)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L8" s="18">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M8" s="15" t="e">
         <f t="shared" si="1"/>
@@ -6351,11 +6684,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="J9" s="18">
-        <f>COUNTIF(Junk!A1:A75,A9)+COUNTIF(Junk!Q1:T75,A9)</f>
+        <f>COUNTIF(Junk!A1:A75,A9)+COUNTIF(Junk!P1:S75,A9)</f>
         <v>0</v>
       </c>
       <c r="K9" s="54" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A9)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A9)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A9)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A9)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L9" s="18">
@@ -6405,16 +6738,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="J10" s="18">
-        <f>COUNTIF(Junk!A1:A75,A10)+COUNTIF(Junk!Q1:T75,A10)</f>
-        <v>0</v>
+        <f>COUNTIF(Junk!A1:A75,A10)+COUNTIF(Junk!P1:S75,A10)</f>
+        <v>2</v>
       </c>
       <c r="K10" s="54" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A10)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A10)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A10)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A10)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L10" s="18">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M10" s="54" t="e">
         <f t="shared" si="1"/>
@@ -6460,16 +6793,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="J11" s="31">
-        <f>COUNTIF(Junk!A1:A75,A11)+COUNTIF(Junk!Q1:T75,A11)</f>
-        <v>1</v>
+        <f>COUNTIF(Junk!A1:A75,A11)+COUNTIF(Junk!P1:S75,A11)</f>
+        <v>0</v>
       </c>
       <c r="K11" s="56" t="e">
-        <f>SUMIFS(Junk!M1:N75,Junk!N1:O75,A11)+SUMIFS(Junk!P1:R75,Junk!Q1:T75,A11)</f>
+        <f>SUMIFS(Junk!M1:N75,Junk!N1:N75,A11)+SUMIFS(Junk!O1:Q75,Junk!P1:S75,A11)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L11" s="31">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M11" s="56" t="e">
         <f t="shared" si="1"/>
@@ -6506,17 +6839,17 @@
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="63" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F13" s="107" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G13" s="108"/>
       <c r="H13" s="109" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I13" s="110"/>
       <c r="J13" s="53"/>
@@ -6534,7 +6867,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="65">
@@ -6576,7 +6909,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="65">
@@ -6618,7 +6951,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="65">
@@ -6660,7 +6993,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C17" s="43"/>
       <c r="D17" s="70">
@@ -6712,7 +7045,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="13"/>
       <c r="N18" s="74" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="O18" s="8"/>
       <c r="P18" s="6" t="s">

</xml_diff>

<commit_message>
Upgraded backgrounds, better snarks, better friend bonuses
</commit_message>
<xml_diff>
--- a/deck.xlsx
+++ b/deck.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Junk" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Primitives" sheetId="2" r:id="rId3"/>
     <sheet name="Stats" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -154,9 +154,6 @@
     <t>Cuddly Baby Blanket</t>
   </si>
   <si>
-    <t>Bundle of Two-by-Fours</t>
-  </si>
-  <si>
     <t>Abandoned Fruit Cart</t>
   </si>
   <si>
@@ -415,36 +412,15 @@
     <t>"What's this sparkly thing? Maybe I can trade it in."</t>
   </si>
   <si>
-    <t>"This would make a nice wagon!"</t>
-  </si>
-  <si>
-    <t>"There's plenty of room in here."</t>
-  </si>
-  <si>
-    <t>"What's up with those colors?"</t>
-  </si>
-  <si>
     <t>"A good find AND a wise business decision!"</t>
   </si>
   <si>
-    <t>"Nobody's gonna mess with me now."</t>
-  </si>
-  <si>
-    <t>"Are these spikes aerodynamic?"</t>
-  </si>
-  <si>
-    <t>"What was this? A carpet?"</t>
-  </si>
-  <si>
     <t>"Nothing says 'scram!' like a man with a flail."</t>
   </si>
   <si>
     <t>"Woah. Wonder what happened here."</t>
   </si>
   <si>
-    <t>"And it doubles as a showcase!"</t>
-  </si>
-  <si>
     <t>"A distraction is as good as a stab."</t>
   </si>
   <si>
@@ -457,9 +433,6 @@
     <t>"Like what Couch Surfers used before the Garbage Wars!"</t>
   </si>
   <si>
-    <t>"These things are useless without the internet."</t>
-  </si>
-  <si>
     <t>"I need a rest, but not that much."</t>
   </si>
   <si>
@@ -469,21 +442,6 @@
     <t>"The gift that keeps on giving. And distracting my enemies."</t>
   </si>
   <si>
-    <t>"Anyone home?"</t>
-  </si>
-  <si>
-    <t>"I don't think that glass will fit"</t>
-  </si>
-  <si>
-    <t>"My lack of wrinkles will give me an edge."</t>
-  </si>
-  <si>
-    <t>"I'm not sure I agree with this artist's worldview."</t>
-  </si>
-  <si>
-    <t>"Look at that lens!"</t>
-  </si>
-  <si>
     <t>"Why do I feel the need to swing on something?"</t>
   </si>
   <si>
@@ -505,9 +463,6 @@
     <t>"Music is a good business plan, right?"</t>
   </si>
   <si>
-    <t>"I can't do anything with this."</t>
-  </si>
-  <si>
     <t>"I qualify as a good cause, right?"</t>
   </si>
   <si>
@@ -538,12 +493,6 @@
     <t>"Clearcutting does have its advantages… for me!"</t>
   </si>
   <si>
-    <t>"Just let the metal come to me. What could go wrong?"</t>
-  </si>
-  <si>
-    <t>"I'll tell people that she needs gas money."</t>
-  </si>
-  <si>
     <t>"Wait, what's a bindle again?"</t>
   </si>
   <si>
@@ -553,36 +502,21 @@
     <t>"I wonder how cyborgs worked during the Steampunk Age."</t>
   </si>
   <si>
-    <t>"What's after post-modern? Caveman. Fashion's cyclical."</t>
-  </si>
-  <si>
     <t>"Now with more  disease!"</t>
   </si>
   <si>
-    <t>"Is 'being green' with a submarine just being blue?"</t>
-  </si>
-  <si>
     <t>"Victory is mine. And now everyone knows it."</t>
   </si>
   <si>
     <t>"Timing is everything."</t>
   </si>
   <si>
-    <t>"Is that a tank?"</t>
-  </si>
-  <si>
     <t>"Great for traversing those Papershred Hills!"</t>
   </si>
   <si>
-    <t>"A bizarre bazaar."</t>
-  </si>
-  <si>
     <t>"Where's my allen wrench?"</t>
   </si>
   <si>
-    <t>"Intimidating and practical!"</t>
-  </si>
-  <si>
     <t>bonus1_num</t>
   </si>
   <si>
@@ -631,27 +565,12 @@
     <t>"Shiny things? I like shiny things."</t>
   </si>
   <si>
-    <t>Hm. I'd rather have him on my side.</t>
-  </si>
-  <si>
     <t>"You must first know thy elements."</t>
   </si>
   <si>
     <t>Seriously - they don't mind!</t>
   </si>
   <si>
-    <t>"Who's got two lungs and a trade skill? This guy."</t>
-  </si>
-  <si>
-    <t>Freddy the Talkative Glassblower</t>
-  </si>
-  <si>
-    <t>Duck Private Gone AWOL</t>
-  </si>
-  <si>
-    <t>Rogue Duck Admiral</t>
-  </si>
-  <si>
     <t>A Wise Hobo</t>
   </si>
   <si>
@@ -670,33 +589,122 @@
     <t>"I eat dirt like you for breakfast!"</t>
   </si>
   <si>
-    <t>"I'll help you today. Then I'm moving on."</t>
-  </si>
-  <si>
     <t>Corrupt Duck Major</t>
   </si>
   <si>
     <t>"Who's going to question a major?"</t>
   </si>
   <si>
-    <t>"Anything can be made out of wood. Anything."</t>
-  </si>
-  <si>
-    <t>"Have you seen my glasses? I can't find my glasses."</t>
-  </si>
-  <si>
     <t>Respected Duck Sergeant</t>
+  </si>
+  <si>
+    <t>"For an immediate initiative arbitration in one of yours' favors…"</t>
+  </si>
+  <si>
+    <t>Pushy Tape Trader</t>
+  </si>
+  <si>
+    <t>Trust me. You want him on your side.</t>
+  </si>
+  <si>
+    <t>"Where I come from, carving is a contact sport."</t>
+  </si>
+  <si>
+    <t>"Did I ever tell you about the time we disabled fourteen flaming barrel mortars?"</t>
+  </si>
+  <si>
+    <t>A Smarmy Rogue</t>
+  </si>
+  <si>
+    <t>Chet the Friendly Glassblower</t>
+  </si>
+  <si>
+    <t>"Why would anyone want a clock in their coffin?"</t>
+  </si>
+  <si>
+    <t>"This must be some sort of pre-historic key chain!!"</t>
+  </si>
+  <si>
+    <t>"Please tell me those colors were never popular."</t>
+  </si>
+  <si>
+    <t>"These spikes don't look very aerodynamic."</t>
+  </si>
+  <si>
+    <t>"What's this? A carpet?"</t>
+  </si>
+  <si>
+    <t>"Who's gonna mess with a guy in this?"</t>
+  </si>
+  <si>
+    <t>"Do you think this is what drove the fish to rebel?"</t>
+  </si>
+  <si>
+    <t>"I'm so glad we trashed these things and used paper instead."</t>
+  </si>
+  <si>
+    <t>"The lack of wrinkles will give me the edge I need!"</t>
+  </si>
+  <si>
+    <t>"What's with all this colored gunk?"</t>
+  </si>
+  <si>
+    <t>"Dear Mother, I am scrapping this desk after I write this letter."</t>
+  </si>
+  <si>
+    <t>"I'll tell people that she's my sister and she needs gas money."</t>
+  </si>
+  <si>
+    <t>"To be clear, we don't sell fleas. They come free."</t>
+  </si>
+  <si>
+    <t>"I don't think that glass will fit."
+"Challenge accepted!"</t>
+  </si>
+  <si>
+    <t>"Anyone home?"
+"Yes?"
+"Can I have it?"</t>
+  </si>
+  <si>
+    <t>"Who's got two lungs and a trade skill??
+This guy."</t>
+  </si>
+  <si>
+    <t>"I don't really know why this one is better than yours. I just know it is."</t>
+  </si>
+  <si>
+    <t>Bundle of 
+Two-by-Fours</t>
+  </si>
+  <si>
+    <t>"Just let the metal come to me. 
+What could go wrong?"</t>
+  </si>
+  <si>
+    <t>"What's after post-modern? 
+Caveman. Fashion is cyclical."</t>
+  </si>
+  <si>
+    <t>"Isn't 'being green' with a submarine just being blue?"</t>
+  </si>
+  <si>
+    <t>"Nobody's gonna miss thes pallets right?"</t>
+  </si>
+  <si>
+    <t>"I shall call him Mort. 
+He will protect me and carry my junk."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1265,7 +1273,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1588,6 +1596,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1607,16 +1627,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3030,21 +3044,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GF58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:R1"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" style="74" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.69921875" style="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.8984375" style="130" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.59765625" style="131" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.59765625" style="131" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.796875" style="132" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5" style="74" customWidth="1"/>
     <col min="7" max="7" width="4.59765625" style="74" customWidth="1"/>
@@ -3060,7 +3074,7 @@
     <col min="189" max="16384" width="6.59765625" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188" s="116" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:188" s="116" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
         <v>0</v>
       </c>
@@ -3071,7 +3085,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="110" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E1" s="111" t="s">
         <v>3</v>
@@ -3086,34 +3100,34 @@
         <v>6</v>
       </c>
       <c r="I1" s="113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J1" s="111" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="K1" s="114" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="L1" s="114" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="M1" s="114" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="N1" s="112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O1" s="112" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="P1" s="112" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="Q1" s="112" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="R1" s="112" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="S1" s="115"/>
       <c r="T1" s="115"/>
@@ -3286,7 +3300,7 @@
       <c r="GE1" s="115"/>
       <c r="GF1" s="115"/>
     </row>
-    <row r="2" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="117" t="s">
         <v>8</v>
       </c>
@@ -3297,7 +3311,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="120" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="121"/>
       <c r="F2" s="122"/>
@@ -3320,7 +3334,7 @@
       <c r="Q2" s="123"/>
       <c r="R2" s="126"/>
     </row>
-    <row r="3" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
@@ -3331,7 +3345,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E3" s="67"/>
       <c r="F3" s="72">
@@ -3356,7 +3370,7 @@
       <c r="Q3" s="72"/>
       <c r="R3" s="73"/>
     </row>
-    <row r="4" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
@@ -3367,7 +3381,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="127" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="72">
@@ -3394,7 +3408,7 @@
       <c r="Q4" s="72"/>
       <c r="R4" s="73"/>
     </row>
-    <row r="5" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64" t="s">
         <v>8</v>
       </c>
@@ -3405,7 +3419,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="127" t="s">
-        <v>133</v>
+        <v>201</v>
       </c>
       <c r="E5" s="70">
         <v>3</v>
@@ -3430,7 +3444,7 @@
       <c r="Q5" s="72"/>
       <c r="R5" s="73"/>
     </row>
-    <row r="6" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="64" t="s">
         <v>8</v>
       </c>
@@ -3441,7 +3455,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="127" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E6" s="67"/>
       <c r="F6" s="68"/>
@@ -3468,7 +3482,7 @@
       <c r="Q6" s="72"/>
       <c r="R6" s="72"/>
     </row>
-    <row r="7" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="64" t="s">
         <v>8</v>
       </c>
@@ -3479,7 +3493,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E7" s="67"/>
       <c r="F7" s="72">
@@ -3508,7 +3522,7 @@
       <c r="Q7" s="72"/>
       <c r="R7" s="72"/>
     </row>
-    <row r="8" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="64" t="s">
         <v>8</v>
       </c>
@@ -3519,7 +3533,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="127" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="E8" s="70">
         <v>2</v>
@@ -3546,7 +3560,7 @@
       <c r="Q8" s="72"/>
       <c r="R8" s="73"/>
     </row>
-    <row r="9" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="64" t="s">
         <v>8</v>
       </c>
@@ -3557,7 +3571,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="127" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E9" s="70">
         <v>2</v>
@@ -3582,7 +3596,7 @@
       <c r="Q9" s="72"/>
       <c r="R9" s="73"/>
     </row>
-    <row r="10" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="64" t="s">
         <v>8</v>
       </c>
@@ -3593,7 +3607,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="127" t="s">
-        <v>136</v>
+        <v>205</v>
       </c>
       <c r="E10" s="70">
         <v>5</v>
@@ -3616,7 +3630,7 @@
       <c r="Q10" s="72"/>
       <c r="R10" s="73"/>
     </row>
-    <row r="11" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="64" t="s">
         <v>8</v>
       </c>
@@ -3627,7 +3641,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="127" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="E11" s="70">
         <v>3</v>
@@ -3652,7 +3666,7 @@
       <c r="Q11" s="72"/>
       <c r="R11" s="73"/>
     </row>
-    <row r="12" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="64" t="s">
         <v>8</v>
       </c>
@@ -3663,7 +3677,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="127" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="E12" s="70">
         <v>2</v>
@@ -3692,7 +3706,7 @@
       <c r="Q12" s="72"/>
       <c r="R12" s="72"/>
     </row>
-    <row r="13" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="64" t="s">
         <v>8</v>
       </c>
@@ -3703,7 +3717,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="127" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E13" s="67"/>
       <c r="F13" s="72">
@@ -3724,7 +3738,7 @@
       <c r="Q13" s="72"/>
       <c r="R13" s="73"/>
     </row>
-    <row r="14" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="64" t="s">
         <v>8</v>
       </c>
@@ -3735,7 +3749,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="127" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E14" s="70">
         <v>2</v>
@@ -3764,7 +3778,7 @@
       <c r="Q14" s="72"/>
       <c r="R14" s="72"/>
     </row>
-    <row r="15" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="64" t="s">
         <v>8</v>
       </c>
@@ -3775,7 +3789,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="127" t="s">
-        <v>141</v>
+        <v>206</v>
       </c>
       <c r="E15" s="67"/>
       <c r="F15" s="72">
@@ -3802,7 +3816,7 @@
       <c r="Q15" s="72"/>
       <c r="R15" s="73"/>
     </row>
-    <row r="16" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="64" t="s">
         <v>8</v>
       </c>
@@ -3813,7 +3827,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="127" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E16" s="67"/>
       <c r="F16" s="72">
@@ -3840,7 +3854,7 @@
       <c r="Q16" s="72"/>
       <c r="R16" s="73"/>
     </row>
-    <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="64" t="s">
         <v>8</v>
       </c>
@@ -3851,7 +3865,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="127" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E17" s="67"/>
       <c r="F17" s="68"/>
@@ -3874,7 +3888,7 @@
       <c r="Q17" s="72"/>
       <c r="R17" s="73"/>
     </row>
-    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="64" t="s">
         <v>8</v>
       </c>
@@ -3885,7 +3899,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="127" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E18" s="70">
         <v>3</v>
@@ -3906,7 +3920,7 @@
       <c r="Q18" s="72"/>
       <c r="R18" s="73"/>
     </row>
-    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="64" t="s">
         <v>8</v>
       </c>
@@ -3917,7 +3931,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="127" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="E19" s="67"/>
       <c r="F19" s="68"/>
@@ -3942,7 +3956,7 @@
       <c r="Q19" s="72"/>
       <c r="R19" s="73"/>
     </row>
-    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="64" t="s">
         <v>8</v>
       </c>
@@ -3953,7 +3967,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="127" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E20" s="67"/>
       <c r="F20" s="72">
@@ -3968,7 +3982,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L20" s="72"/>
       <c r="M20" s="71"/>
@@ -3978,7 +3992,7 @@
       <c r="Q20" s="72"/>
       <c r="R20" s="72"/>
     </row>
-    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="64" t="s">
         <v>8</v>
       </c>
@@ -3989,7 +4003,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="127" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E21" s="70">
         <v>4</v>
@@ -4010,7 +4024,7 @@
       <c r="Q21" s="72"/>
       <c r="R21" s="73"/>
     </row>
-    <row r="22" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="64" t="s">
         <v>8</v>
       </c>
@@ -4021,7 +4035,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="127" t="s">
-        <v>151</v>
+        <v>213</v>
       </c>
       <c r="E22" s="70">
         <v>2</v>
@@ -4048,7 +4062,7 @@
       <c r="Q22" s="72"/>
       <c r="R22" s="73"/>
     </row>
-    <row r="23" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="64" t="s">
         <v>8</v>
       </c>
@@ -4059,7 +4073,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="127" t="s">
-        <v>150</v>
+        <v>214</v>
       </c>
       <c r="E23" s="70">
         <v>3</v>
@@ -4082,7 +4096,7 @@
       <c r="Q23" s="72"/>
       <c r="R23" s="73"/>
     </row>
-    <row r="24" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="64" t="s">
         <v>8</v>
       </c>
@@ -4093,7 +4107,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="127" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="E24" s="70">
         <v>3</v>
@@ -4120,7 +4134,7 @@
       <c r="Q24" s="72"/>
       <c r="R24" s="73"/>
     </row>
-    <row r="25" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="64" t="s">
         <v>8</v>
       </c>
@@ -4131,7 +4145,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="127" t="s">
-        <v>153</v>
+        <v>209</v>
       </c>
       <c r="E25" s="70">
         <v>2</v>
@@ -4154,7 +4168,7 @@
       <c r="Q25" s="72"/>
       <c r="R25" s="73"/>
     </row>
-    <row r="26" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="64" t="s">
         <v>8</v>
       </c>
@@ -4165,7 +4179,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="127" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="E26" s="70">
         <v>2</v>
@@ -4190,7 +4204,7 @@
       <c r="Q26" s="72"/>
       <c r="R26" s="73"/>
     </row>
-    <row r="27" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="64" t="s">
         <v>8</v>
       </c>
@@ -4201,7 +4215,7 @@
         <v>43</v>
       </c>
       <c r="D27" s="127" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="E27" s="67"/>
       <c r="F27" s="68"/>
@@ -4222,7 +4236,7 @@
       <c r="Q27" s="72"/>
       <c r="R27" s="73"/>
     </row>
-    <row r="28" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="64" t="s">
         <v>8</v>
       </c>
@@ -4233,7 +4247,7 @@
         <v>43</v>
       </c>
       <c r="D28" s="127" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="E28" s="70">
         <v>5</v>
@@ -4256,18 +4270,18 @@
       <c r="Q28" s="72"/>
       <c r="R28" s="73"/>
     </row>
-    <row r="29" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="65" t="s">
-        <v>45</v>
+      <c r="B29" s="145" t="s">
+        <v>217</v>
       </c>
       <c r="C29" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D29" s="127" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E29" s="70">
         <v>2</v>
@@ -4292,18 +4306,18 @@
       <c r="Q29" s="72"/>
       <c r="R29" s="73"/>
     </row>
-    <row r="30" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="127" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="E30" s="67"/>
       <c r="F30" s="72">
@@ -4328,18 +4342,18 @@
       <c r="Q30" s="72"/>
       <c r="R30" s="73"/>
     </row>
-    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D31" s="127" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E31" s="70">
         <v>1</v>
@@ -4366,18 +4380,18 @@
       <c r="Q31" s="72"/>
       <c r="R31" s="73"/>
     </row>
-    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="127" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E32" s="70">
         <v>3</v>
@@ -4402,18 +4416,18 @@
       <c r="Q32" s="72"/>
       <c r="R32" s="73"/>
     </row>
-    <row r="33" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D33" s="127" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="E33" s="67"/>
       <c r="F33" s="72">
@@ -4438,18 +4452,18 @@
       <c r="Q33" s="72"/>
       <c r="R33" s="73"/>
     </row>
-    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D34" s="127" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="E34" s="70">
         <v>3</v>
@@ -4472,18 +4486,18 @@
       <c r="Q34" s="72"/>
       <c r="R34" s="73"/>
     </row>
-    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="127" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="E35" s="70">
         <v>2</v>
@@ -4506,18 +4520,18 @@
       <c r="Q35" s="72"/>
       <c r="R35" s="73"/>
     </row>
-    <row r="36" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="65" t="s">
         <v>52</v>
-      </c>
-      <c r="B36" s="65" t="s">
-        <v>53</v>
       </c>
       <c r="C36" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="127" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E36" s="67"/>
       <c r="F36" s="68"/>
@@ -4546,18 +4560,18 @@
       <c r="Q36" s="72"/>
       <c r="R36" s="72"/>
     </row>
-    <row r="37" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="127" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E37" s="67"/>
       <c r="F37" s="72">
@@ -4586,18 +4600,18 @@
       <c r="Q37" s="72"/>
       <c r="R37" s="72"/>
     </row>
-    <row r="38" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="127" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E38" s="67"/>
       <c r="F38" s="72">
@@ -4628,18 +4642,18 @@
       <c r="Q38" s="72"/>
       <c r="R38" s="72"/>
     </row>
-    <row r="39" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="127" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E39" s="70">
         <v>2</v>
@@ -4670,18 +4684,18 @@
       <c r="Q39" s="72"/>
       <c r="R39" s="72"/>
     </row>
-    <row r="40" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="40" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="127" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="E40" s="67"/>
       <c r="F40" s="68"/>
@@ -4708,18 +4722,18 @@
       <c r="Q40" s="72"/>
       <c r="R40" s="72"/>
     </row>
-    <row r="41" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="41" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="127" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E41" s="70">
         <v>2</v>
@@ -4737,13 +4751,13 @@
       <c r="L41" s="129"/>
       <c r="M41" s="68"/>
       <c r="N41" s="129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O41" s="72">
         <v>1</v>
       </c>
       <c r="P41" s="73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q41" s="72">
         <v>1</v>
@@ -4752,18 +4766,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="127" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E42" s="70">
         <v>2</v>
@@ -4781,13 +4795,13 @@
       <c r="L42" s="129"/>
       <c r="M42" s="68"/>
       <c r="N42" s="129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O42" s="72">
         <v>1</v>
       </c>
       <c r="P42" s="73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q42" s="72">
         <v>1</v>
@@ -4796,18 +4810,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="43" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="127" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E43" s="67"/>
       <c r="F43" s="68"/>
@@ -4834,18 +4848,18 @@
       <c r="Q43" s="72"/>
       <c r="R43" s="73"/>
     </row>
-    <row r="44" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="44" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="127" t="s">
-        <v>173</v>
+        <v>218</v>
       </c>
       <c r="E44" s="67"/>
       <c r="F44" s="72">
@@ -4872,18 +4886,18 @@
       <c r="Q44" s="72"/>
       <c r="R44" s="73"/>
     </row>
-    <row r="45" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="127" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="E45" s="70">
         <v>4</v>
@@ -4908,18 +4922,18 @@
       <c r="Q45" s="72"/>
       <c r="R45" s="73"/>
     </row>
-    <row r="46" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="46" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" s="77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="127" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E46" s="70">
         <v>4</v>
@@ -4942,18 +4956,18 @@
       <c r="Q46" s="72"/>
       <c r="R46" s="73"/>
     </row>
-    <row r="47" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="47" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="127" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="E47" s="70">
         <v>2</v>
@@ -4982,18 +4996,18 @@
       <c r="Q47" s="72"/>
       <c r="R47" s="72"/>
     </row>
-    <row r="48" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="48" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" s="77" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D48" s="127" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="E48" s="70">
         <v>12</v>
@@ -5008,7 +5022,7 @@
       </c>
       <c r="J48" s="67"/>
       <c r="K48" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L48" s="68"/>
       <c r="M48" s="68"/>
@@ -5018,18 +5032,18 @@
       <c r="Q48" s="72"/>
       <c r="R48" s="73"/>
     </row>
-    <row r="49" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="49" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" s="77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="127" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="E49" s="67"/>
       <c r="F49" s="72">
@@ -5044,7 +5058,7 @@
       </c>
       <c r="J49" s="67"/>
       <c r="K49" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L49" s="68"/>
       <c r="M49" s="68"/>
@@ -5054,18 +5068,18 @@
       <c r="Q49" s="72"/>
       <c r="R49" s="73"/>
     </row>
-    <row r="50" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="50" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" s="65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="127" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="E50" s="70">
         <v>12</v>
@@ -5080,7 +5094,7 @@
       </c>
       <c r="J50" s="67"/>
       <c r="K50" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L50" s="68"/>
       <c r="M50" s="68"/>
@@ -5090,18 +5104,18 @@
       <c r="Q50" s="72"/>
       <c r="R50" s="73"/>
     </row>
-    <row r="51" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="51" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="127" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="E51" s="67"/>
       <c r="F51" s="68"/>
@@ -5116,7 +5130,7 @@
       </c>
       <c r="J51" s="67"/>
       <c r="K51" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L51" s="68"/>
       <c r="M51" s="68"/>
@@ -5126,18 +5140,18 @@
       <c r="Q51" s="72"/>
       <c r="R51" s="73"/>
     </row>
-    <row r="52" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="52" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="127" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="E52" s="67"/>
       <c r="F52" s="72">
@@ -5152,7 +5166,7 @@
       </c>
       <c r="J52" s="67"/>
       <c r="K52" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L52" s="68"/>
       <c r="M52" s="68"/>
@@ -5162,18 +5176,18 @@
       <c r="Q52" s="72"/>
       <c r="R52" s="73"/>
     </row>
-    <row r="53" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="53" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D53" s="127" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="E53" s="70">
         <v>2</v>
@@ -5202,18 +5216,18 @@
       <c r="Q53" s="72"/>
       <c r="R53" s="72"/>
     </row>
-    <row r="54" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="54" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D54" s="127" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="E54" s="67"/>
       <c r="F54" s="68"/>
@@ -5240,18 +5254,18 @@
       <c r="Q54" s="72"/>
       <c r="R54" s="72"/>
     </row>
-    <row r="55" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="55" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C55" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D55" s="127" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="E55" s="67"/>
       <c r="F55" s="72">
@@ -5278,18 +5292,18 @@
       <c r="Q55" s="72"/>
       <c r="R55" s="72"/>
     </row>
-    <row r="56" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="56" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" s="65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D56" s="127" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="E56" s="70">
         <v>2</v>
@@ -5309,33 +5323,33 @@
       <c r="L56" s="72"/>
       <c r="M56" s="68"/>
       <c r="N56" s="72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O56" s="72">
         <v>1</v>
       </c>
       <c r="P56" s="73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q56" s="72">
         <v>1</v>
       </c>
       <c r="R56" s="73" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="17.100000000000001" customHeight="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D57" s="127" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="E57" s="67"/>
       <c r="F57" s="68"/>
@@ -5358,18 +5372,18 @@
       <c r="Q57" s="72"/>
       <c r="R57" s="73"/>
     </row>
-    <row r="58" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="58" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C58" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D58" s="127" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="E58" s="67"/>
       <c r="F58" s="72">
@@ -5426,19 +5440,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IK16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.796875" style="89" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.09765625" style="89" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.3984375" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.8984375" style="143" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.8984375" style="137" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.8984375" style="89" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.09765625" style="89" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.8984375" style="89" bestFit="1" customWidth="1"/>
@@ -5452,7 +5466,7 @@
     <col min="18" max="16384" width="8.796875" style="89"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:245" s="107" customFormat="1" ht="15">
+    <row r="1" spans="1:245" s="107" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
@@ -5462,61 +5476,61 @@
       <c r="C1" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="141" t="s">
-        <v>129</v>
+      <c r="D1" s="135" t="s">
+        <v>128</v>
       </c>
       <c r="E1" s="107" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="F1" s="107" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="G1" s="107" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="H1" s="107" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="I1" s="111" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="J1" s="114" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="K1" s="114" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="L1" s="114" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="M1" s="112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N1" s="112" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="O1" s="112" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="P1" s="112" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q1" s="112" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="79" t="s">
         <v>194</v>
-      </c>
-      <c r="Q1" s="112" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1">
-      <c r="A2" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>209</v>
       </c>
       <c r="C2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="140" t="s">
-        <v>201</v>
+      <c r="D2" s="134" t="s">
+        <v>179</v>
       </c>
       <c r="E2" s="81"/>
       <c r="F2" s="82"/>
@@ -5527,13 +5541,13 @@
       <c r="K2" s="86"/>
       <c r="L2" s="82"/>
       <c r="M2" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N2" s="86">
         <v>2</v>
       </c>
       <c r="O2" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P2" s="86">
         <v>1</v>
@@ -5770,18 +5784,18 @@
       <c r="IJ2" s="88"/>
       <c r="IK2" s="88"/>
     </row>
-    <row r="3" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="C3" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="140" t="s">
-        <v>216</v>
+      <c r="D3" s="134" t="s">
+        <v>189</v>
       </c>
       <c r="E3" s="84">
         <v>1</v>
@@ -5800,13 +5814,13 @@
       <c r="K3" s="86"/>
       <c r="L3" s="82"/>
       <c r="M3" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N3" s="86">
         <v>1</v>
       </c>
       <c r="O3" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P3" s="86">
         <v>1</v>
@@ -6043,18 +6057,18 @@
       <c r="IJ3" s="88"/>
       <c r="IK3" s="88"/>
     </row>
-    <row r="4" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C4" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="140" t="s">
-        <v>202</v>
+      <c r="D4" s="134" t="s">
+        <v>180</v>
       </c>
       <c r="E4" s="84">
         <v>1</v>
@@ -6073,13 +6087,13 @@
       <c r="K4" s="86"/>
       <c r="L4" s="82"/>
       <c r="M4" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N4" s="86">
         <v>1</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P4" s="86">
         <v>1</v>
@@ -6316,18 +6330,18 @@
       <c r="IJ4" s="88"/>
       <c r="IK4" s="88"/>
     </row>
-    <row r="5" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="79" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" s="79" t="s">
-        <v>81</v>
       </c>
       <c r="C5" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="140" t="s">
-        <v>203</v>
+      <c r="D5" s="134" t="s">
+        <v>181</v>
       </c>
       <c r="E5" s="84">
         <v>1</v>
@@ -6342,13 +6356,13 @@
       <c r="K5" s="86"/>
       <c r="L5" s="82"/>
       <c r="M5" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N5" s="86">
         <v>1</v>
       </c>
       <c r="O5" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P5" s="86">
         <v>2</v>
@@ -6585,18 +6599,18 @@
       <c r="IJ5" s="88"/>
       <c r="IK5" s="88"/>
     </row>
-    <row r="6" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="140" t="s">
-        <v>204</v>
+      <c r="D6" s="134" t="s">
+        <v>195</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="82"/>
@@ -6844,18 +6858,18 @@
       <c r="IJ6" s="88"/>
       <c r="IK6" s="88"/>
     </row>
-    <row r="7" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="79" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="C7" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="140" t="s">
-        <v>205</v>
+      <c r="D7" s="134" t="s">
+        <v>182</v>
       </c>
       <c r="E7" s="84">
         <v>2</v>
@@ -6870,7 +6884,7 @@
       <c r="K7" s="86"/>
       <c r="L7" s="82"/>
       <c r="M7" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N7" s="86">
         <v>1</v>
@@ -7113,18 +7127,18 @@
       <c r="IJ7" s="88"/>
       <c r="IK7" s="88"/>
     </row>
-    <row r="8" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="140" t="s">
-        <v>206</v>
+      <c r="D8" s="134" t="s">
+        <v>183</v>
       </c>
       <c r="E8" s="81"/>
       <c r="F8" s="82"/>
@@ -7372,18 +7386,18 @@
       <c r="IJ8" s="88"/>
       <c r="IK8" s="88"/>
     </row>
-    <row r="9" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C9" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="140" t="s">
-        <v>207</v>
+      <c r="D9" s="144" t="s">
+        <v>215</v>
       </c>
       <c r="E9" s="84">
         <v>3</v>
@@ -7398,7 +7412,7 @@
       <c r="K9" s="86"/>
       <c r="L9" s="82"/>
       <c r="M9" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N9" s="86">
         <v>1</v>
@@ -7410,7 +7424,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R9" s="88"/>
       <c r="S9" s="88"/>
@@ -7641,18 +7655,18 @@
       <c r="IJ9" s="88"/>
       <c r="IK9" s="88"/>
     </row>
-    <row r="10" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="140" t="s">
-        <v>212</v>
+      <c r="D10" s="134" t="s">
+        <v>185</v>
       </c>
       <c r="E10" s="84">
         <v>1</v>
@@ -7666,7 +7680,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="90" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="K10" s="86"/>
       <c r="L10" s="85"/>
@@ -7904,18 +7918,18 @@
       <c r="IJ10" s="88"/>
       <c r="IK10" s="88"/>
     </row>
-    <row r="11" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="140" t="s">
-        <v>214</v>
+      <c r="D11" s="134" t="s">
+        <v>187</v>
       </c>
       <c r="E11" s="84">
         <v>2</v>
@@ -8171,18 +8185,18 @@
       <c r="IJ11" s="88"/>
       <c r="IK11" s="88"/>
     </row>
-    <row r="12" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="140" t="s">
-        <v>215</v>
+      <c r="D12" s="134" t="s">
+        <v>188</v>
       </c>
       <c r="E12" s="84">
         <v>2</v>
@@ -8197,19 +8211,19 @@
       <c r="K12" s="86"/>
       <c r="L12" s="82"/>
       <c r="M12" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N12" s="86">
         <v>1</v>
       </c>
       <c r="O12" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P12" s="86">
         <v>1</v>
       </c>
       <c r="Q12" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R12" s="88"/>
       <c r="S12" s="88"/>
@@ -8440,18 +8454,18 @@
       <c r="IJ12" s="88"/>
       <c r="IK12" s="88"/>
     </row>
-    <row r="13" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="140" t="s">
-        <v>217</v>
+      <c r="D13" s="134" t="s">
+        <v>193</v>
       </c>
       <c r="E13" s="93"/>
       <c r="F13" s="82"/>
@@ -8459,7 +8473,7 @@
       <c r="H13" s="83"/>
       <c r="I13" s="84"/>
       <c r="J13" s="85" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="K13" s="87"/>
       <c r="L13" s="94"/>
@@ -8697,18 +8711,18 @@
       <c r="IJ13" s="88"/>
       <c r="IK13" s="88"/>
     </row>
-    <row r="14" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C14" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="140" t="s">
-        <v>219</v>
+      <c r="D14" s="134" t="s">
+        <v>191</v>
       </c>
       <c r="E14" s="84">
         <v>1</v>
@@ -8723,13 +8737,13 @@
       <c r="K14" s="86"/>
       <c r="L14" s="85"/>
       <c r="M14" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N14" s="86">
         <v>1</v>
       </c>
       <c r="O14" s="86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P14" s="86">
         <v>1</v>
@@ -8966,18 +8980,18 @@
       <c r="IJ14" s="88"/>
       <c r="IK14" s="88"/>
     </row>
-    <row r="15" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C15" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="140" t="s">
-        <v>220</v>
+      <c r="D15" s="134" t="s">
+        <v>196</v>
       </c>
       <c r="E15" s="84">
         <v>2</v>
@@ -8992,7 +9006,7 @@
       <c r="K15" s="86"/>
       <c r="L15" s="94"/>
       <c r="M15" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N15" s="86">
         <v>1</v>
@@ -9004,7 +9018,7 @@
         <v>1</v>
       </c>
       <c r="Q15" s="87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R15" s="88"/>
       <c r="S15" s="88"/>
@@ -9235,18 +9249,18 @@
       <c r="IJ15" s="88"/>
       <c r="IK15" s="88"/>
     </row>
-    <row r="16" spans="1:245" s="106" customFormat="1" ht="15.75" customHeight="1">
+    <row r="16" spans="1:245" s="106" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="142" t="s">
-        <v>221</v>
+      <c r="D16" s="136" t="s">
+        <v>197</v>
       </c>
       <c r="E16" s="100">
         <v>1</v>
@@ -9526,12 +9540,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.59765625" style="23" customWidth="1"/>
     <col min="2" max="2" width="9" style="23" customWidth="1"/>
@@ -9540,7 +9554,7 @@
     <col min="5" max="256" width="6.59765625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
@@ -9548,295 +9562,295 @@
         <v>0</v>
       </c>
       <c r="C1" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="B2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>98</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>102</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="29"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="6"/>
@@ -9851,14 +9865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.3984375" style="35" customWidth="1"/>
     <col min="2" max="2" width="6.8984375" style="35" customWidth="1"/>
@@ -9876,28 +9890,28 @@
     <col min="15" max="256" width="6.59765625" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1">
-      <c r="A1" s="138" t="s">
+    <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="142" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="139"/>
+      <c r="C1" s="138" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="134" t="s">
+      <c r="D1" s="143"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="138" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="139"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="134" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="135"/>
-      <c r="H1" s="134" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" s="135"/>
-      <c r="J1" s="134" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="135"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="138" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="139"/>
       <c r="L1" s="29"/>
       <c r="M1" s="11"/>
       <c r="N1" s="36"/>
@@ -9906,7 +9920,7 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9914,37 +9928,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="N2" s="37"/>
       <c r="O2" s="6"/>
@@ -9952,7 +9966,7 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="str">
         <f>Primitives!A3</f>
         <v>initiative</v>
@@ -9990,7 +10004,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
     </row>
-    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>Primitives!A4</f>
         <v>capacity</v>
@@ -10028,7 +10042,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="17"/>
       <c r="C5" s="16"/>
@@ -10060,7 +10074,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="str">
         <f>Primitives!A20</f>
         <v>take one</v>
@@ -10098,7 +10112,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="str">
         <f>Primitives!A24</f>
         <v>string</v>
@@ -10152,7 +10166,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>Primitives!A25</f>
         <v>wood</v>
@@ -10207,7 +10221,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>Primitives!A23</f>
         <v>metal</v>
@@ -10262,7 +10276,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -10316,7 +10330,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="str">
         <f>Primitives!A21</f>
         <v>duct tape</v>
@@ -10371,7 +10385,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="16.5" customHeight="1">
+    <row r="12" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="48"/>
       <c r="C12" s="49"/>
@@ -10391,24 +10405,24 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="F13" s="138" t="s">
         <v>122</v>
       </c>
-      <c r="F13" s="134" t="s">
+      <c r="G13" s="139"/>
+      <c r="H13" s="140" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="135"/>
-      <c r="H13" s="136" t="s">
-        <v>124</v>
-      </c>
-      <c r="I13" s="137"/>
+      <c r="I13" s="141"/>
       <c r="J13" s="42"/>
       <c r="K13" s="9"/>
       <c r="L13" s="6"/>
@@ -10419,12 +10433,12 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="54">
@@ -10461,12 +10475,12 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="54">
@@ -10503,12 +10517,12 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="54">
@@ -10545,12 +10559,12 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1">
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="59">
@@ -10587,7 +10601,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -10602,7 +10616,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="11"/>
       <c r="N18" s="63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="4" t="s">
@@ -10615,7 +10629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -10646,7 +10660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -10674,7 +10688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>

</xml_diff>

<commit_message>
Fixing the snark height thing.
</commit_message>
<xml_diff>
--- a/deck.xlsx
+++ b/deck.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Junk" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Primitives" sheetId="2" r:id="rId3"/>
     <sheet name="Stats" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -674,10 +674,6 @@
     <t>"I don't really know why this one is better than yours. I just know it is."</t>
   </si>
   <si>
-    <t>Bundle of 
-Two-by-Fours</t>
-  </si>
-  <si>
     <t>"Just let the metal come to me. 
 What could go wrong?"</t>
   </si>
@@ -694,17 +690,20 @@
   <si>
     <t>"I shall call him Mort. 
 He will protect me and carry my junk."</t>
+  </si>
+  <si>
+    <t>Bundle of Two-by-Fours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1608,6 +1607,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1625,12 +1630,6 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3044,16 +3043,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:GF58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.5" style="74" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.69921875" style="74" bestFit="1" customWidth="1"/>
@@ -3074,7 +3073,7 @@
     <col min="189" max="16384" width="6.59765625" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188" s="116" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:188" s="116" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="108" t="s">
         <v>0</v>
       </c>
@@ -3300,7 +3299,7 @@
       <c r="GE1" s="115"/>
       <c r="GF1" s="115"/>
     </row>
-    <row r="2" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="117" t="s">
         <v>8</v>
       </c>
@@ -3334,7 +3333,7 @@
       <c r="Q2" s="123"/>
       <c r="R2" s="126"/>
     </row>
-    <row r="3" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
@@ -3370,7 +3369,7 @@
       <c r="Q3" s="72"/>
       <c r="R3" s="73"/>
     </row>
-    <row r="4" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
@@ -3408,7 +3407,7 @@
       <c r="Q4" s="72"/>
       <c r="R4" s="73"/>
     </row>
-    <row r="5" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="64" t="s">
         <v>8</v>
       </c>
@@ -3444,7 +3443,7 @@
       <c r="Q5" s="72"/>
       <c r="R5" s="73"/>
     </row>
-    <row r="6" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="64" t="s">
         <v>8</v>
       </c>
@@ -3482,7 +3481,7 @@
       <c r="Q6" s="72"/>
       <c r="R6" s="72"/>
     </row>
-    <row r="7" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="64" t="s">
         <v>8</v>
       </c>
@@ -3522,7 +3521,7 @@
       <c r="Q7" s="72"/>
       <c r="R7" s="72"/>
     </row>
-    <row r="8" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="64" t="s">
         <v>8</v>
       </c>
@@ -3560,7 +3559,7 @@
       <c r="Q8" s="72"/>
       <c r="R8" s="73"/>
     </row>
-    <row r="9" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="64" t="s">
         <v>8</v>
       </c>
@@ -3596,7 +3595,7 @@
       <c r="Q9" s="72"/>
       <c r="R9" s="73"/>
     </row>
-    <row r="10" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="64" t="s">
         <v>8</v>
       </c>
@@ -3630,7 +3629,7 @@
       <c r="Q10" s="72"/>
       <c r="R10" s="73"/>
     </row>
-    <row r="11" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="64" t="s">
         <v>8</v>
       </c>
@@ -3666,7 +3665,7 @@
       <c r="Q11" s="72"/>
       <c r="R11" s="73"/>
     </row>
-    <row r="12" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="64" t="s">
         <v>8</v>
       </c>
@@ -3706,7 +3705,7 @@
       <c r="Q12" s="72"/>
       <c r="R12" s="72"/>
     </row>
-    <row r="13" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="64" t="s">
         <v>8</v>
       </c>
@@ -3738,7 +3737,7 @@
       <c r="Q13" s="72"/>
       <c r="R13" s="73"/>
     </row>
-    <row r="14" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="64" t="s">
         <v>8</v>
       </c>
@@ -3778,7 +3777,7 @@
       <c r="Q14" s="72"/>
       <c r="R14" s="72"/>
     </row>
-    <row r="15" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="64" t="s">
         <v>8</v>
       </c>
@@ -3816,7 +3815,7 @@
       <c r="Q15" s="72"/>
       <c r="R15" s="73"/>
     </row>
-    <row r="16" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="64" t="s">
         <v>8</v>
       </c>
@@ -3854,7 +3853,7 @@
       <c r="Q16" s="72"/>
       <c r="R16" s="73"/>
     </row>
-    <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="64" t="s">
         <v>8</v>
       </c>
@@ -3888,7 +3887,7 @@
       <c r="Q17" s="72"/>
       <c r="R17" s="73"/>
     </row>
-    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="64" t="s">
         <v>8</v>
       </c>
@@ -3920,7 +3919,7 @@
       <c r="Q18" s="72"/>
       <c r="R18" s="73"/>
     </row>
-    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="64" t="s">
         <v>8</v>
       </c>
@@ -3956,7 +3955,7 @@
       <c r="Q19" s="72"/>
       <c r="R19" s="73"/>
     </row>
-    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="64" t="s">
         <v>8</v>
       </c>
@@ -3992,7 +3991,7 @@
       <c r="Q20" s="72"/>
       <c r="R20" s="72"/>
     </row>
-    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="64" t="s">
         <v>8</v>
       </c>
@@ -4024,7 +4023,7 @@
       <c r="Q21" s="72"/>
       <c r="R21" s="73"/>
     </row>
-    <row r="22" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="64" t="s">
         <v>8</v>
       </c>
@@ -4062,7 +4061,7 @@
       <c r="Q22" s="72"/>
       <c r="R22" s="73"/>
     </row>
-    <row r="23" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="64" t="s">
         <v>8</v>
       </c>
@@ -4096,7 +4095,7 @@
       <c r="Q23" s="72"/>
       <c r="R23" s="73"/>
     </row>
-    <row r="24" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="64" t="s">
         <v>8</v>
       </c>
@@ -4134,7 +4133,7 @@
       <c r="Q24" s="72"/>
       <c r="R24" s="73"/>
     </row>
-    <row r="25" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="64" t="s">
         <v>8</v>
       </c>
@@ -4168,7 +4167,7 @@
       <c r="Q25" s="72"/>
       <c r="R25" s="73"/>
     </row>
-    <row r="26" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="64" t="s">
         <v>8</v>
       </c>
@@ -4204,7 +4203,7 @@
       <c r="Q26" s="72"/>
       <c r="R26" s="73"/>
     </row>
-    <row r="27" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="64" t="s">
         <v>8</v>
       </c>
@@ -4236,7 +4235,7 @@
       <c r="Q27" s="72"/>
       <c r="R27" s="73"/>
     </row>
-    <row r="28" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="64" t="s">
         <v>8</v>
       </c>
@@ -4270,12 +4269,12 @@
       <c r="Q28" s="72"/>
       <c r="R28" s="73"/>
     </row>
-    <row r="29" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="145" t="s">
-        <v>217</v>
+      <c r="B29" s="139" t="s">
+        <v>222</v>
       </c>
       <c r="C29" s="66" t="s">
         <v>43</v>
@@ -4306,7 +4305,7 @@
       <c r="Q29" s="72"/>
       <c r="R29" s="73"/>
     </row>
-    <row r="30" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="64" t="s">
         <v>8</v>
       </c>
@@ -4342,7 +4341,7 @@
       <c r="Q30" s="72"/>
       <c r="R30" s="73"/>
     </row>
-    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="64" t="s">
         <v>8</v>
       </c>
@@ -4380,7 +4379,7 @@
       <c r="Q31" s="72"/>
       <c r="R31" s="73"/>
     </row>
-    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="64" t="s">
         <v>8</v>
       </c>
@@ -4416,7 +4415,7 @@
       <c r="Q32" s="72"/>
       <c r="R32" s="73"/>
     </row>
-    <row r="33" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="64" t="s">
         <v>8</v>
       </c>
@@ -4452,7 +4451,7 @@
       <c r="Q33" s="72"/>
       <c r="R33" s="73"/>
     </row>
-    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="64" t="s">
         <v>8</v>
       </c>
@@ -4486,7 +4485,7 @@
       <c r="Q34" s="72"/>
       <c r="R34" s="73"/>
     </row>
-    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="64" t="s">
         <v>8</v>
       </c>
@@ -4520,7 +4519,7 @@
       <c r="Q35" s="72"/>
       <c r="R35" s="73"/>
     </row>
-    <row r="36" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="64" t="s">
         <v>51</v>
       </c>
@@ -4560,7 +4559,7 @@
       <c r="Q36" s="72"/>
       <c r="R36" s="72"/>
     </row>
-    <row r="37" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="64" t="s">
         <v>51</v>
       </c>
@@ -4600,7 +4599,7 @@
       <c r="Q37" s="72"/>
       <c r="R37" s="72"/>
     </row>
-    <row r="38" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="64" t="s">
         <v>51</v>
       </c>
@@ -4642,7 +4641,7 @@
       <c r="Q38" s="72"/>
       <c r="R38" s="72"/>
     </row>
-    <row r="39" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="64" t="s">
         <v>51</v>
       </c>
@@ -4684,7 +4683,7 @@
       <c r="Q39" s="72"/>
       <c r="R39" s="72"/>
     </row>
-    <row r="40" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="64" t="s">
         <v>51</v>
       </c>
@@ -4722,7 +4721,7 @@
       <c r="Q40" s="72"/>
       <c r="R40" s="72"/>
     </row>
-    <row r="41" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="64" t="s">
         <v>51</v>
       </c>
@@ -4766,7 +4765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="64" t="s">
         <v>51</v>
       </c>
@@ -4810,7 +4809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="64" t="s">
         <v>51</v>
       </c>
@@ -4848,7 +4847,7 @@
       <c r="Q43" s="72"/>
       <c r="R43" s="73"/>
     </row>
-    <row r="44" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="64" t="s">
         <v>51</v>
       </c>
@@ -4859,7 +4858,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="127" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E44" s="67"/>
       <c r="F44" s="72">
@@ -4886,7 +4885,7 @@
       <c r="Q44" s="72"/>
       <c r="R44" s="73"/>
     </row>
-    <row r="45" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="64" t="s">
         <v>51</v>
       </c>
@@ -4922,7 +4921,7 @@
       <c r="Q45" s="72"/>
       <c r="R45" s="73"/>
     </row>
-    <row r="46" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="64" t="s">
         <v>51</v>
       </c>
@@ -4956,7 +4955,7 @@
       <c r="Q46" s="72"/>
       <c r="R46" s="73"/>
     </row>
-    <row r="47" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="64" t="s">
         <v>51</v>
       </c>
@@ -4996,7 +4995,7 @@
       <c r="Q47" s="72"/>
       <c r="R47" s="72"/>
     </row>
-    <row r="48" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="64" t="s">
         <v>51</v>
       </c>
@@ -5032,7 +5031,7 @@
       <c r="Q48" s="72"/>
       <c r="R48" s="73"/>
     </row>
-    <row r="49" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="64" t="s">
         <v>51</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>10</v>
       </c>
       <c r="D49" s="127" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E49" s="67"/>
       <c r="F49" s="72">
@@ -5068,7 +5067,7 @@
       <c r="Q49" s="72"/>
       <c r="R49" s="73"/>
     </row>
-    <row r="50" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="64" t="s">
         <v>51</v>
       </c>
@@ -5104,7 +5103,7 @@
       <c r="Q50" s="72"/>
       <c r="R50" s="73"/>
     </row>
-    <row r="51" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="64" t="s">
         <v>51</v>
       </c>
@@ -5115,7 +5114,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="127" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E51" s="67"/>
       <c r="F51" s="68"/>
@@ -5140,7 +5139,7 @@
       <c r="Q51" s="72"/>
       <c r="R51" s="73"/>
     </row>
-    <row r="52" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="64" t="s">
         <v>51</v>
       </c>
@@ -5176,7 +5175,7 @@
       <c r="Q52" s="72"/>
       <c r="R52" s="73"/>
     </row>
-    <row r="53" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="64" t="s">
         <v>51</v>
       </c>
@@ -5216,7 +5215,7 @@
       <c r="Q53" s="72"/>
       <c r="R53" s="72"/>
     </row>
-    <row r="54" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="64" t="s">
         <v>51</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>43</v>
       </c>
       <c r="D54" s="127" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E54" s="67"/>
       <c r="F54" s="68"/>
@@ -5254,7 +5253,7 @@
       <c r="Q54" s="72"/>
       <c r="R54" s="72"/>
     </row>
-    <row r="55" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="64" t="s">
         <v>51</v>
       </c>
@@ -5292,7 +5291,7 @@
       <c r="Q55" s="72"/>
       <c r="R55" s="72"/>
     </row>
-    <row r="56" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="64" t="s">
         <v>51</v>
       </c>
@@ -5338,7 +5337,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="64" t="s">
         <v>51</v>
       </c>
@@ -5372,7 +5371,7 @@
       <c r="Q57" s="72"/>
       <c r="R57" s="73"/>
     </row>
-    <row r="58" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A58" s="64" t="s">
         <v>51</v>
       </c>
@@ -5383,7 +5382,7 @@
         <v>43</v>
       </c>
       <c r="D58" s="127" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E58" s="67"/>
       <c r="F58" s="72">
@@ -5440,14 +5439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IK16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.796875" style="89" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.09765625" style="89" bestFit="1" customWidth="1"/>
@@ -5466,7 +5465,7 @@
     <col min="18" max="16384" width="8.796875" style="89"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:245" s="107" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:245" s="107" customFormat="1" ht="15">
       <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="78" t="s">
         <v>79</v>
       </c>
@@ -5784,7 +5783,7 @@
       <c r="IJ2" s="88"/>
       <c r="IK2" s="88"/>
     </row>
-    <row r="3" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="78" t="s">
         <v>79</v>
       </c>
@@ -6057,7 +6056,7 @@
       <c r="IJ3" s="88"/>
       <c r="IK3" s="88"/>
     </row>
-    <row r="4" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="78" t="s">
         <v>79</v>
       </c>
@@ -6330,7 +6329,7 @@
       <c r="IJ4" s="88"/>
       <c r="IK4" s="88"/>
     </row>
-    <row r="5" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="78" t="s">
         <v>79</v>
       </c>
@@ -6599,7 +6598,7 @@
       <c r="IJ5" s="88"/>
       <c r="IK5" s="88"/>
     </row>
-    <row r="6" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>79</v>
       </c>
@@ -6858,7 +6857,7 @@
       <c r="IJ6" s="88"/>
       <c r="IK6" s="88"/>
     </row>
-    <row r="7" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="78" t="s">
         <v>79</v>
       </c>
@@ -7127,7 +7126,7 @@
       <c r="IJ7" s="88"/>
       <c r="IK7" s="88"/>
     </row>
-    <row r="8" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="78" t="s">
         <v>79</v>
       </c>
@@ -7386,7 +7385,7 @@
       <c r="IJ8" s="88"/>
       <c r="IK8" s="88"/>
     </row>
-    <row r="9" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="78" t="s">
         <v>79</v>
       </c>
@@ -7396,7 +7395,7 @@
       <c r="C9" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="144" t="s">
+      <c r="D9" s="138" t="s">
         <v>215</v>
       </c>
       <c r="E9" s="84">
@@ -7655,7 +7654,7 @@
       <c r="IJ9" s="88"/>
       <c r="IK9" s="88"/>
     </row>
-    <row r="10" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="78" t="s">
         <v>79</v>
       </c>
@@ -7918,7 +7917,7 @@
       <c r="IJ10" s="88"/>
       <c r="IK10" s="88"/>
     </row>
-    <row r="11" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="78" t="s">
         <v>79</v>
       </c>
@@ -8185,7 +8184,7 @@
       <c r="IJ11" s="88"/>
       <c r="IK11" s="88"/>
     </row>
-    <row r="12" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="78" t="s">
         <v>79</v>
       </c>
@@ -8454,7 +8453,7 @@
       <c r="IJ12" s="88"/>
       <c r="IK12" s="88"/>
     </row>
-    <row r="13" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="78" t="s">
         <v>79</v>
       </c>
@@ -8711,7 +8710,7 @@
       <c r="IJ13" s="88"/>
       <c r="IK13" s="88"/>
     </row>
-    <row r="14" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="78" t="s">
         <v>79</v>
       </c>
@@ -8980,7 +8979,7 @@
       <c r="IJ14" s="88"/>
       <c r="IK14" s="88"/>
     </row>
-    <row r="15" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="78" t="s">
         <v>79</v>
       </c>
@@ -9249,7 +9248,7 @@
       <c r="IJ15" s="88"/>
       <c r="IK15" s="88"/>
     </row>
-    <row r="16" spans="1:245" s="106" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:245" s="106" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="97" t="s">
         <v>79</v>
       </c>
@@ -9540,12 +9539,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.59765625" style="23" customWidth="1"/>
     <col min="2" max="2" width="9" style="23" customWidth="1"/>
@@ -9554,7 +9553,7 @@
     <col min="5" max="256" width="6.59765625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
@@ -9569,7 +9568,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="26" t="s">
         <v>95</v>
       </c>
@@ -9582,7 +9581,7 @@
       <c r="D2" s="28"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -9595,7 +9594,7 @@
       <c r="D3" s="29"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -9608,7 +9607,7 @@
       <c r="D4" s="29"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>100</v>
       </c>
@@ -9621,7 +9620,7 @@
       <c r="D5" s="29"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -9634,7 +9633,7 @@
       <c r="D6" s="29"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>66</v>
       </c>
@@ -9645,7 +9644,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>60</v>
       </c>
@@ -9656,7 +9655,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>58</v>
       </c>
@@ -9667,7 +9666,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>76</v>
       </c>
@@ -9678,7 +9677,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -9689,7 +9688,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>85</v>
       </c>
@@ -9700,7 +9699,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>83</v>
       </c>
@@ -9711,7 +9710,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>91</v>
       </c>
@@ -9722,7 +9721,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>90</v>
       </c>
@@ -9733,7 +9732,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>103</v>
       </c>
@@ -9744,7 +9743,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
@@ -9755,7 +9754,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -9766,7 +9765,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -9777,7 +9776,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>11</v>
       </c>
@@ -9790,7 +9789,7 @@
       <c r="D20" s="32"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="33" t="s">
         <v>7</v>
       </c>
@@ -9803,7 +9802,7 @@
       <c r="D21" s="34"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
@@ -9816,7 +9815,7 @@
       <c r="D22" s="29"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -9829,7 +9828,7 @@
       <c r="D23" s="29"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
@@ -9842,7 +9841,7 @@
       <c r="D24" s="29"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
@@ -9865,14 +9864,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.3984375" style="35" customWidth="1"/>
     <col min="2" max="2" width="6.8984375" style="35" customWidth="1"/>
@@ -9890,28 +9889,28 @@
     <col min="15" max="256" width="6.59765625" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="142" t="s">
+    <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1">
+      <c r="A1" s="144" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="138" t="s">
+      <c r="B1" s="141"/>
+      <c r="C1" s="140" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="143"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="138" t="s">
+      <c r="D1" s="145"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="138" t="s">
+      <c r="G1" s="141"/>
+      <c r="H1" s="140" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="139"/>
-      <c r="J1" s="138" t="s">
+      <c r="I1" s="141"/>
+      <c r="J1" s="140" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="139"/>
+      <c r="K1" s="141"/>
       <c r="L1" s="29"/>
       <c r="M1" s="11"/>
       <c r="N1" s="36"/>
@@ -9920,7 +9919,7 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9966,7 +9965,7 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="38" t="str">
         <f>Primitives!A3</f>
         <v>initiative</v>
@@ -10004,7 +10003,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
     </row>
-    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="4" t="str">
         <f>Primitives!A4</f>
         <v>capacity</v>
@@ -10042,7 +10041,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="17"/>
       <c r="C5" s="16"/>
@@ -10074,7 +10073,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="44" t="str">
         <f>Primitives!A20</f>
         <v>take one</v>
@@ -10112,7 +10111,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="38" t="str">
         <f>Primitives!A24</f>
         <v>string</v>
@@ -10166,7 +10165,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="4" t="str">
         <f>Primitives!A25</f>
         <v>wood</v>
@@ -10221,7 +10220,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="4" t="str">
         <f>Primitives!A23</f>
         <v>metal</v>
@@ -10276,7 +10275,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -10330,7 +10329,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11" s="44" t="str">
         <f>Primitives!A21</f>
         <v>duct tape</v>
@@ -10385,7 +10384,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="16.5" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="48"/>
       <c r="C12" s="49"/>
@@ -10405,7 +10404,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -10415,14 +10414,14 @@
       <c r="E13" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="138" t="s">
+      <c r="F13" s="140" t="s">
         <v>122</v>
       </c>
-      <c r="G13" s="139"/>
-      <c r="H13" s="140" t="s">
+      <c r="G13" s="141"/>
+      <c r="H13" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="I13" s="141"/>
+      <c r="I13" s="143"/>
       <c r="J13" s="42"/>
       <c r="K13" s="9"/>
       <c r="L13" s="6"/>
@@ -10433,7 +10432,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -10475,7 +10474,7 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -10517,7 +10516,7 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -10559,7 +10558,7 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15.75" customHeight="1">
       <c r="A17" s="44" t="s">
         <v>6</v>
       </c>
@@ -10601,7 +10600,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15.75" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -10629,7 +10628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -10660,7 +10659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -10688,7 +10687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>

</xml_diff>